<commit_message>
-recopying .gb links directly from FreeGenes into the package as before I manipulated them myself
</commit_message>
<xml_diff>
--- a/Open Enzymes Collection/Open Enzymes Collection.xlsx
+++ b/Open Enzymes Collection/Open Enzymes Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Open Enzymes Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D52CEB-8E16-A840-81BF-388F26002D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDCF4C7-E278-F34C-A185-8EA1857B25FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -23824,7 +23824,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23878,16 +23878,17 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -24339,8 +24340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24414,14 +24415,14 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="52" t="s">
         <v>7618</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -24666,7 +24667,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="49" t="s">
         <v>7532</v>
       </c>
       <c r="B15" s="41" t="s">
@@ -24678,13 +24679,13 @@
       <c r="D15" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="49" t="s">
         <v>7619</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="55" t="s">
         <v>7697</v>
       </c>
       <c r="H15" s="18"/>
@@ -24704,7 +24705,7 @@
       <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="50" t="s">
         <v>7533</v>
       </c>
       <c r="B16" s="41" t="s">
@@ -24716,13 +24717,13 @@
       <c r="D16" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E16" s="52" t="s">
+      <c r="E16" s="49" t="s">
         <v>7620</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="55" t="s">
         <v>7698</v>
       </c>
       <c r="H16" s="18"/>
@@ -24742,7 +24743,7 @@
       <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="50" t="s">
         <v>7534</v>
       </c>
       <c r="B17" s="41" t="s">
@@ -24754,13 +24755,13 @@
       <c r="D17" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="49" t="s">
         <v>7621</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="55" t="s">
         <v>7699</v>
       </c>
       <c r="H17" s="18"/>
@@ -24780,7 +24781,7 @@
       <c r="M17" s="22"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="50" t="s">
         <v>7535</v>
       </c>
       <c r="B18" s="41" t="s">
@@ -24792,13 +24793,13 @@
       <c r="D18" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="49" t="s">
         <v>7622</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="55" t="s">
         <v>7700</v>
       </c>
       <c r="H18" s="18"/>
@@ -24818,7 +24819,7 @@
       <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="49" t="s">
         <v>7536</v>
       </c>
       <c r="B19" s="41" t="s">
@@ -24830,13 +24831,13 @@
       <c r="D19" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="49" t="s">
         <v>7623</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="55" t="s">
         <v>7701</v>
       </c>
       <c r="H19" s="18"/>
@@ -24856,7 +24857,7 @@
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="50" t="s">
         <v>7537</v>
       </c>
       <c r="B20" s="41" t="s">
@@ -24868,13 +24869,13 @@
       <c r="D20" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E20" s="52" t="s">
+      <c r="E20" s="49" t="s">
         <v>7624</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="55" t="s">
         <v>7702</v>
       </c>
       <c r="H20" s="18"/>
@@ -24894,7 +24895,7 @@
       <c r="M20" s="21"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="49" t="s">
         <v>7538</v>
       </c>
       <c r="B21" s="41" t="s">
@@ -24906,13 +24907,13 @@
       <c r="D21" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E21" s="52" t="s">
+      <c r="E21" s="49" t="s">
         <v>7625</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="55" t="s">
         <v>7703</v>
       </c>
       <c r="H21" s="18"/>
@@ -24932,7 +24933,7 @@
       <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="49" t="s">
         <v>7539</v>
       </c>
       <c r="B22" s="41" t="s">
@@ -24944,13 +24945,13 @@
       <c r="D22" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E22" s="52" t="s">
+      <c r="E22" s="49" t="s">
         <v>7626</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="55" t="s">
         <v>7704</v>
       </c>
       <c r="H22" s="18"/>
@@ -24970,7 +24971,7 @@
       <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="49" t="s">
         <v>7540</v>
       </c>
       <c r="B23" s="41" t="s">
@@ -24982,13 +24983,13 @@
       <c r="D23" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="51" t="s">
         <v>7627</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="55" t="s">
         <v>7705</v>
       </c>
       <c r="H23" s="18"/>
@@ -25008,7 +25009,7 @@
       <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="52" t="s">
+      <c r="A24" s="49" t="s">
         <v>7541</v>
       </c>
       <c r="B24" s="41" t="s">
@@ -25020,13 +25021,13 @@
       <c r="D24" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="51" t="s">
         <v>7628</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="55" t="s">
         <v>7706</v>
       </c>
       <c r="H24" s="18"/>
@@ -25046,7 +25047,7 @@
       <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="49" t="s">
         <v>7542</v>
       </c>
       <c r="B25" s="41" t="s">
@@ -25058,13 +25059,13 @@
       <c r="D25" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E25" s="52" t="s">
+      <c r="E25" s="49" t="s">
         <v>7629</v>
       </c>
       <c r="F25" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="55" t="s">
         <v>7707</v>
       </c>
       <c r="H25" s="18"/>
@@ -25084,7 +25085,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="49" t="s">
         <v>7543</v>
       </c>
       <c r="B26" s="41" t="s">
@@ -25096,13 +25097,13 @@
       <c r="D26" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E26" s="54" t="s">
+      <c r="E26" s="51" t="s">
         <v>7630</v>
       </c>
       <c r="F26" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="55" t="s">
         <v>7708</v>
       </c>
       <c r="H26" s="18"/>
@@ -25122,7 +25123,7 @@
       <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="49" t="s">
         <v>7544</v>
       </c>
       <c r="B27" s="41" t="s">
@@ -25134,13 +25135,13 @@
       <c r="D27" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="E27" s="51" t="s">
         <v>7631</v>
       </c>
       <c r="F27" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="G27" s="55" t="s">
         <v>7709</v>
       </c>
       <c r="H27" s="18"/>
@@ -25160,7 +25161,7 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="52" t="s">
+      <c r="A28" s="49" t="s">
         <v>7545</v>
       </c>
       <c r="B28" s="41" t="s">
@@ -25172,13 +25173,13 @@
       <c r="D28" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E28" s="52" t="s">
+      <c r="E28" s="49" t="s">
         <v>7632</v>
       </c>
       <c r="F28" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G28" s="21" t="s">
+      <c r="G28" s="55" t="s">
         <v>7710</v>
       </c>
       <c r="H28" s="18"/>
@@ -25198,7 +25199,7 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="52" t="s">
+      <c r="A29" s="49" t="s">
         <v>7546</v>
       </c>
       <c r="B29" s="41" t="s">
@@ -25210,13 +25211,13 @@
       <c r="D29" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E29" s="52" t="s">
+      <c r="E29" s="49" t="s">
         <v>7633</v>
       </c>
       <c r="F29" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="55" t="s">
         <v>7711</v>
       </c>
       <c r="H29" s="18"/>
@@ -25236,7 +25237,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="49" t="s">
         <v>7547</v>
       </c>
       <c r="B30" s="41" t="s">
@@ -25248,13 +25249,13 @@
       <c r="D30" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E30" s="52" t="s">
+      <c r="E30" s="49" t="s">
         <v>7634</v>
       </c>
       <c r="F30" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G30" s="55" t="s">
         <v>7712</v>
       </c>
       <c r="H30" s="18"/>
@@ -25274,7 +25275,7 @@
       <c r="M30" s="23"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="49" t="s">
         <v>7548</v>
       </c>
       <c r="B31" s="41" t="s">
@@ -25286,13 +25287,13 @@
       <c r="D31" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E31" s="52" t="s">
+      <c r="E31" s="49" t="s">
         <v>7635</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G31" s="21" t="s">
+      <c r="G31" s="55" t="s">
         <v>7713</v>
       </c>
       <c r="H31" s="18"/>
@@ -25312,7 +25313,7 @@
       <c r="M31" s="23"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="49" t="s">
         <v>7549</v>
       </c>
       <c r="B32" s="41" t="s">
@@ -25324,13 +25325,13 @@
       <c r="D32" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="49" t="s">
         <v>7636</v>
       </c>
       <c r="F32" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="G32" s="55" t="s">
         <v>7714</v>
       </c>
       <c r="H32" s="18"/>
@@ -25350,7 +25351,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="49" t="s">
         <v>7550</v>
       </c>
       <c r="B33" s="41" t="s">
@@ -25362,13 +25363,13 @@
       <c r="D33" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E33" s="52" t="s">
+      <c r="E33" s="49" t="s">
         <v>7637</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G33" s="21" t="s">
+      <c r="G33" s="55" t="s">
         <v>7715</v>
       </c>
       <c r="H33" s="18"/>
@@ -25388,7 +25389,7 @@
       <c r="M33" s="24"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A34" s="52" t="s">
+      <c r="A34" s="49" t="s">
         <v>7551</v>
       </c>
       <c r="B34" s="41" t="s">
@@ -25400,13 +25401,13 @@
       <c r="D34" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E34" s="52" t="s">
+      <c r="E34" s="49" t="s">
         <v>7638</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="G34" s="55" t="s">
         <v>7716</v>
       </c>
       <c r="H34" s="18"/>
@@ -25426,7 +25427,7 @@
       <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="52" t="s">
+      <c r="A35" s="49" t="s">
         <v>7552</v>
       </c>
       <c r="B35" s="41" t="s">
@@ -25438,13 +25439,13 @@
       <c r="D35" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E35" s="52" t="s">
+      <c r="E35" s="49" t="s">
         <v>7639</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="55" t="s">
         <v>7717</v>
       </c>
       <c r="H35" s="18"/>
@@ -25464,7 +25465,7 @@
       <c r="M35" s="21"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="49" t="s">
         <v>7553</v>
       </c>
       <c r="B36" s="41" t="s">
@@ -25476,13 +25477,13 @@
       <c r="D36" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E36" s="52" t="s">
+      <c r="E36" s="49" t="s">
         <v>7640</v>
       </c>
       <c r="F36" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="G36" s="55" t="s">
         <v>7718</v>
       </c>
       <c r="H36" s="18"/>
@@ -25502,7 +25503,7 @@
       <c r="M36" s="21"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="52" t="s">
+      <c r="A37" s="49" t="s">
         <v>7554</v>
       </c>
       <c r="B37" s="41" t="s">
@@ -25514,13 +25515,13 @@
       <c r="D37" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E37" s="52" t="s">
+      <c r="E37" s="49" t="s">
         <v>7641</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G37" s="21" t="s">
+      <c r="G37" s="55" t="s">
         <v>7719</v>
       </c>
       <c r="H37" s="18"/>
@@ -25540,7 +25541,7 @@
       <c r="M37" s="21"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="49" t="s">
         <v>7555</v>
       </c>
       <c r="B38" s="41" t="s">
@@ -25552,13 +25553,13 @@
       <c r="D38" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E38" s="52" t="s">
+      <c r="E38" s="49" t="s">
         <v>7642</v>
       </c>
       <c r="F38" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G38" s="21" t="s">
+      <c r="G38" s="55" t="s">
         <v>7720</v>
       </c>
       <c r="H38" s="18"/>
@@ -25578,7 +25579,7 @@
       <c r="M38" s="21"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="49" t="s">
         <v>7556</v>
       </c>
       <c r="B39" s="41" t="s">
@@ -25590,13 +25591,13 @@
       <c r="D39" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E39" s="52" t="s">
+      <c r="E39" s="49" t="s">
         <v>7643</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G39" s="21" t="s">
+      <c r="G39" s="55" t="s">
         <v>7721</v>
       </c>
       <c r="H39" s="18"/>
@@ -25610,13 +25611,13 @@
         <v>1</v>
       </c>
       <c r="L39" s="15">
-        <f t="shared" ref="L39:L96" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M39,CHAR(160)," ")," ",""))))</f>
+        <f t="shared" ref="L39:L95" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M39,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
       </c>
       <c r="M39" s="21"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A40" s="52" t="s">
+      <c r="A40" s="49" t="s">
         <v>7557</v>
       </c>
       <c r="B40" s="41" t="s">
@@ -25628,13 +25629,13 @@
       <c r="D40" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E40" s="52" t="s">
+      <c r="E40" s="49" t="s">
         <v>7644</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G40" s="55" t="s">
         <v>7722</v>
       </c>
       <c r="H40" s="18"/>
@@ -25654,7 +25655,7 @@
       <c r="M40" s="21"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A41" s="52" t="s">
+      <c r="A41" s="49" t="s">
         <v>7558</v>
       </c>
       <c r="B41" s="41" t="s">
@@ -25666,13 +25667,13 @@
       <c r="D41" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E41" s="52" t="s">
+      <c r="E41" s="49" t="s">
         <v>7645</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="55" t="s">
         <v>7723</v>
       </c>
       <c r="H41" s="18"/>
@@ -25692,7 +25693,7 @@
       <c r="M41" s="21"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A42" s="52" t="s">
+      <c r="A42" s="49" t="s">
         <v>7559</v>
       </c>
       <c r="B42" s="41" t="s">
@@ -25704,13 +25705,13 @@
       <c r="D42" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E42" s="52" t="s">
+      <c r="E42" s="49" t="s">
         <v>7646</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G42" s="21" t="s">
+      <c r="G42" s="55" t="s">
         <v>7724</v>
       </c>
       <c r="H42" s="18"/>
@@ -25730,7 +25731,7 @@
       <c r="M42" s="21"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A43" s="52" t="s">
+      <c r="A43" s="49" t="s">
         <v>7560</v>
       </c>
       <c r="B43" s="41" t="s">
@@ -25742,13 +25743,13 @@
       <c r="D43" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E43" s="52" t="s">
+      <c r="E43" s="49" t="s">
         <v>7647</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="55" t="s">
         <v>7725</v>
       </c>
       <c r="H43" s="18"/>
@@ -25768,7 +25769,7 @@
       <c r="M43" s="21"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A44" s="52" t="s">
+      <c r="A44" s="49" t="s">
         <v>7561</v>
       </c>
       <c r="B44" s="41" t="s">
@@ -25780,13 +25781,13 @@
       <c r="D44" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E44" s="52" t="s">
+      <c r="E44" s="49" t="s">
         <v>7648</v>
       </c>
       <c r="F44" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G44" s="21" t="s">
+      <c r="G44" s="55" t="s">
         <v>7726</v>
       </c>
       <c r="H44" s="18"/>
@@ -25806,7 +25807,7 @@
       <c r="M44" s="21"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A45" s="52" t="s">
+      <c r="A45" s="49" t="s">
         <v>7562</v>
       </c>
       <c r="B45" s="41" t="s">
@@ -25818,13 +25819,13 @@
       <c r="D45" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E45" s="52" t="s">
+      <c r="E45" s="49" t="s">
         <v>7649</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G45" s="21" t="s">
+      <c r="G45" s="55" t="s">
         <v>7727</v>
       </c>
       <c r="H45" s="18"/>
@@ -25844,7 +25845,7 @@
       <c r="M45" s="21"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A46" s="52" t="s">
+      <c r="A46" s="49" t="s">
         <v>7563</v>
       </c>
       <c r="B46" s="41" t="s">
@@ -25856,13 +25857,13 @@
       <c r="D46" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E46" s="52" t="s">
+      <c r="E46" s="49" t="s">
         <v>7650</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="G46" s="55" t="s">
         <v>7728</v>
       </c>
       <c r="H46" s="18"/>
@@ -25882,7 +25883,7 @@
       <c r="M46" s="21"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A47" s="52" t="s">
+      <c r="A47" s="49" t="s">
         <v>7564</v>
       </c>
       <c r="B47" s="41" t="s">
@@ -25894,13 +25895,13 @@
       <c r="D47" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E47" s="52" t="s">
+      <c r="E47" s="49" t="s">
         <v>7564</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="55" t="s">
         <v>7729</v>
       </c>
       <c r="H47" s="18"/>
@@ -25920,7 +25921,7 @@
       <c r="M47" s="21"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A48" s="52" t="s">
+      <c r="A48" s="49" t="s">
         <v>7565</v>
       </c>
       <c r="B48" s="41" t="s">
@@ -25932,13 +25933,13 @@
       <c r="D48" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E48" s="52" t="s">
+      <c r="E48" s="49" t="s">
         <v>7565</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="G48" s="55" t="s">
         <v>7730</v>
       </c>
       <c r="H48" s="18"/>
@@ -25958,7 +25959,7 @@
       <c r="M48" s="21"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A49" s="52" t="s">
+      <c r="A49" s="49" t="s">
         <v>7566</v>
       </c>
       <c r="B49" s="41" t="s">
@@ -25970,13 +25971,13 @@
       <c r="D49" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E49" s="52" t="s">
+      <c r="E49" s="49" t="s">
         <v>7651</v>
       </c>
       <c r="F49" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="G49" s="55" t="s">
         <v>7731</v>
       </c>
       <c r="H49" s="18"/>
@@ -25996,7 +25997,7 @@
       <c r="M49" s="21"/>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A50" s="52" t="s">
+      <c r="A50" s="49" t="s">
         <v>7567</v>
       </c>
       <c r="B50" s="41" t="s">
@@ -26008,13 +26009,13 @@
       <c r="D50" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E50" s="52" t="s">
+      <c r="E50" s="49" t="s">
         <v>7652</v>
       </c>
       <c r="F50" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="G50" s="55" t="s">
         <v>7732</v>
       </c>
       <c r="H50" s="18"/>
@@ -26034,7 +26035,7 @@
       <c r="M50" s="21"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A51" s="52" t="s">
+      <c r="A51" s="49" t="s">
         <v>7568</v>
       </c>
       <c r="B51" s="41" t="s">
@@ -26046,13 +26047,13 @@
       <c r="D51" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E51" s="52" t="s">
+      <c r="E51" s="49" t="s">
         <v>7653</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="G51" s="55" t="s">
         <v>7733</v>
       </c>
       <c r="H51" s="18"/>
@@ -26072,7 +26073,7 @@
       <c r="M51" s="21"/>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A52" s="52" t="s">
+      <c r="A52" s="49" t="s">
         <v>7569</v>
       </c>
       <c r="B52" s="41" t="s">
@@ -26084,13 +26085,13 @@
       <c r="D52" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E52" s="52" t="s">
+      <c r="E52" s="49" t="s">
         <v>7654</v>
       </c>
       <c r="F52" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="G52" s="55" t="s">
         <v>7734</v>
       </c>
       <c r="H52" s="18"/>
@@ -26110,7 +26111,7 @@
       <c r="M52" s="21"/>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A53" s="52" t="s">
+      <c r="A53" s="49" t="s">
         <v>7570</v>
       </c>
       <c r="B53" s="41" t="s">
@@ -26122,13 +26123,13 @@
       <c r="D53" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E53" s="52" t="s">
+      <c r="E53" s="49" t="s">
         <v>7655</v>
       </c>
       <c r="F53" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="G53" s="55" t="s">
         <v>7735</v>
       </c>
       <c r="H53" s="18"/>
@@ -26148,7 +26149,7 @@
       <c r="M53" s="21"/>
     </row>
     <row r="54" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A54" s="52" t="s">
+      <c r="A54" s="49" t="s">
         <v>7571</v>
       </c>
       <c r="B54" s="41" t="s">
@@ -26160,13 +26161,13 @@
       <c r="D54" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E54" s="52" t="s">
+      <c r="E54" s="49" t="s">
         <v>7656</v>
       </c>
       <c r="F54" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="G54" s="55" t="s">
         <v>7736</v>
       </c>
       <c r="H54" s="18"/>
@@ -26186,7 +26187,7 @@
       <c r="M54" s="21"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A55" s="52" t="s">
+      <c r="A55" s="49" t="s">
         <v>7572</v>
       </c>
       <c r="B55" s="41" t="s">
@@ -26198,13 +26199,13 @@
       <c r="D55" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E55" s="52" t="s">
+      <c r="E55" s="49" t="s">
         <v>7657</v>
       </c>
       <c r="F55" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G55" s="21" t="s">
+      <c r="G55" s="55" t="s">
         <v>7737</v>
       </c>
       <c r="H55" s="18"/>
@@ -26224,7 +26225,7 @@
       <c r="M55" s="21"/>
     </row>
     <row r="56" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A56" s="52" t="s">
+      <c r="A56" s="49" t="s">
         <v>7573</v>
       </c>
       <c r="B56" s="41" t="s">
@@ -26236,13 +26237,13 @@
       <c r="D56" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E56" s="52" t="s">
+      <c r="E56" s="49" t="s">
         <v>7658</v>
       </c>
       <c r="F56" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G56" s="21" t="s">
+      <c r="G56" s="55" t="s">
         <v>7738</v>
       </c>
       <c r="H56" s="18"/>
@@ -26262,7 +26263,7 @@
       <c r="M56" s="21"/>
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A57" s="52" t="s">
+      <c r="A57" s="49" t="s">
         <v>7574</v>
       </c>
       <c r="B57" s="41" t="s">
@@ -26274,13 +26275,13 @@
       <c r="D57" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E57" s="52" t="s">
+      <c r="E57" s="49" t="s">
         <v>7659</v>
       </c>
       <c r="F57" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G57" s="21" t="s">
+      <c r="G57" s="55" t="s">
         <v>7739</v>
       </c>
       <c r="H57" s="18"/>
@@ -26300,7 +26301,7 @@
       <c r="M57" s="21"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A58" s="52" t="s">
+      <c r="A58" s="49" t="s">
         <v>7575</v>
       </c>
       <c r="B58" s="41" t="s">
@@ -26312,13 +26313,13 @@
       <c r="D58" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E58" s="52" t="s">
+      <c r="E58" s="49" t="s">
         <v>7660</v>
       </c>
       <c r="F58" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G58" s="21" t="s">
+      <c r="G58" s="55" t="s">
         <v>7740</v>
       </c>
       <c r="H58" s="18"/>
@@ -26338,7 +26339,7 @@
       <c r="M58" s="21"/>
     </row>
     <row r="59" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A59" s="52" t="s">
+      <c r="A59" s="49" t="s">
         <v>7576</v>
       </c>
       <c r="B59" s="41" t="s">
@@ -26350,13 +26351,13 @@
       <c r="D59" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E59" s="52" t="s">
+      <c r="E59" s="49" t="s">
         <v>7661</v>
       </c>
       <c r="F59" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G59" s="21" t="s">
+      <c r="G59" s="55" t="s">
         <v>7741</v>
       </c>
       <c r="H59" s="18"/>
@@ -26376,7 +26377,7 @@
       <c r="M59" s="21"/>
     </row>
     <row r="60" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A60" s="52" t="s">
+      <c r="A60" s="49" t="s">
         <v>7577</v>
       </c>
       <c r="B60" s="41" t="s">
@@ -26388,13 +26389,13 @@
       <c r="D60" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E60" s="52" t="s">
+      <c r="E60" s="49" t="s">
         <v>7662</v>
       </c>
       <c r="F60" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G60" s="21" t="s">
+      <c r="G60" s="55" t="s">
         <v>7742</v>
       </c>
       <c r="H60" s="18"/>
@@ -26414,7 +26415,7 @@
       <c r="M60" s="21"/>
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A61" s="52" t="s">
+      <c r="A61" s="49" t="s">
         <v>7578</v>
       </c>
       <c r="B61" s="41" t="s">
@@ -26426,13 +26427,13 @@
       <c r="D61" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E61" s="52" t="s">
+      <c r="E61" s="49" t="s">
         <v>7663</v>
       </c>
       <c r="F61" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G61" s="21" t="s">
+      <c r="G61" s="55" t="s">
         <v>7743</v>
       </c>
       <c r="H61" s="18"/>
@@ -26452,7 +26453,7 @@
       <c r="M61" s="21"/>
     </row>
     <row r="62" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A62" s="52" t="s">
+      <c r="A62" s="49" t="s">
         <v>7579</v>
       </c>
       <c r="B62" s="41" t="s">
@@ -26464,13 +26465,13 @@
       <c r="D62" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E62" s="52" t="s">
+      <c r="E62" s="49" t="s">
         <v>7664</v>
       </c>
       <c r="F62" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G62" s="21" t="s">
+      <c r="G62" s="55" t="s">
         <v>7744</v>
       </c>
       <c r="H62" s="18"/>
@@ -26490,7 +26491,7 @@
       <c r="M62" s="21"/>
     </row>
     <row r="63" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A63" s="52" t="s">
+      <c r="A63" s="49" t="s">
         <v>7580</v>
       </c>
       <c r="B63" s="41" t="s">
@@ -26502,13 +26503,13 @@
       <c r="D63" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E63" s="52" t="s">
+      <c r="E63" s="49" t="s">
         <v>7665</v>
       </c>
       <c r="F63" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G63" s="21" t="s">
+      <c r="G63" s="55" t="s">
         <v>7745</v>
       </c>
       <c r="H63" s="18"/>
@@ -26528,7 +26529,7 @@
       <c r="M63" s="21"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A64" s="52" t="s">
+      <c r="A64" s="49" t="s">
         <v>7581</v>
       </c>
       <c r="B64" s="41" t="s">
@@ -26540,13 +26541,13 @@
       <c r="D64" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E64" s="52" t="s">
+      <c r="E64" s="49" t="s">
         <v>7666</v>
       </c>
       <c r="F64" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G64" s="21" t="s">
+      <c r="G64" s="55" t="s">
         <v>7746</v>
       </c>
       <c r="H64" s="18"/>
@@ -26566,7 +26567,7 @@
       <c r="M64" s="21"/>
     </row>
     <row r="65" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A65" s="52" t="s">
+      <c r="A65" s="49" t="s">
         <v>7582</v>
       </c>
       <c r="B65" s="41" t="s">
@@ -26578,13 +26579,13 @@
       <c r="D65" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E65" s="52" t="s">
+      <c r="E65" s="49" t="s">
         <v>7667</v>
       </c>
       <c r="F65" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G65" s="21" t="s">
+      <c r="G65" s="55" t="s">
         <v>7747</v>
       </c>
       <c r="H65" s="18"/>
@@ -26604,7 +26605,7 @@
       <c r="M65" s="21"/>
     </row>
     <row r="66" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A66" s="52" t="s">
+      <c r="A66" s="49" t="s">
         <v>7583</v>
       </c>
       <c r="B66" s="41" t="s">
@@ -26616,13 +26617,13 @@
       <c r="D66" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E66" s="52" t="s">
+      <c r="E66" s="49" t="s">
         <v>7668</v>
       </c>
       <c r="F66" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G66" s="21" t="s">
+      <c r="G66" s="55" t="s">
         <v>7748</v>
       </c>
       <c r="H66" s="18"/>
@@ -26642,7 +26643,7 @@
       <c r="M66" s="21"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A67" s="52" t="s">
+      <c r="A67" s="49" t="s">
         <v>7584</v>
       </c>
       <c r="B67" s="41" t="s">
@@ -26654,13 +26655,13 @@
       <c r="D67" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E67" s="52" t="s">
+      <c r="E67" s="49" t="s">
         <v>7669</v>
       </c>
       <c r="F67" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G67" s="21" t="s">
+      <c r="G67" s="55" t="s">
         <v>7749</v>
       </c>
       <c r="H67" s="18"/>
@@ -26680,7 +26681,7 @@
       <c r="M67" s="21"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A68" s="52" t="s">
+      <c r="A68" s="49" t="s">
         <v>7585</v>
       </c>
       <c r="B68" s="41" t="s">
@@ -26692,13 +26693,13 @@
       <c r="D68" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E68" s="52" t="s">
+      <c r="E68" s="49" t="s">
         <v>7670</v>
       </c>
       <c r="F68" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G68" s="21" t="s">
+      <c r="G68" s="55" t="s">
         <v>7750</v>
       </c>
       <c r="H68" s="18"/>
@@ -26718,7 +26719,7 @@
       <c r="M68" s="21"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A69" s="52" t="s">
+      <c r="A69" s="49" t="s">
         <v>7586</v>
       </c>
       <c r="B69" s="41" t="s">
@@ -26730,13 +26731,13 @@
       <c r="D69" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E69" s="52" t="s">
+      <c r="E69" s="49" t="s">
         <v>7671</v>
       </c>
       <c r="F69" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G69" s="21" t="s">
+      <c r="G69" s="55" t="s">
         <v>7751</v>
       </c>
       <c r="H69" s="18"/>
@@ -26756,7 +26757,7 @@
       <c r="M69" s="21"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A70" s="52" t="s">
+      <c r="A70" s="49" t="s">
         <v>7587</v>
       </c>
       <c r="B70" s="41" t="s">
@@ -26768,13 +26769,13 @@
       <c r="D70" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E70" s="52" t="s">
+      <c r="E70" s="49" t="s">
         <v>7672</v>
       </c>
       <c r="F70" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G70" s="21" t="s">
+      <c r="G70" s="55" t="s">
         <v>7752</v>
       </c>
       <c r="H70" s="18"/>
@@ -26794,7 +26795,7 @@
       <c r="M70" s="21"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A71" s="52" t="s">
+      <c r="A71" s="49" t="s">
         <v>7588</v>
       </c>
       <c r="B71" s="41" t="s">
@@ -26806,13 +26807,13 @@
       <c r="D71" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E71" s="52" t="s">
+      <c r="E71" s="49" t="s">
         <v>7673</v>
       </c>
       <c r="F71" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G71" s="21" t="s">
+      <c r="G71" s="55" t="s">
         <v>7753</v>
       </c>
       <c r="H71" s="18"/>
@@ -26832,7 +26833,7 @@
       <c r="M71" s="21"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A72" s="52" t="s">
+      <c r="A72" s="49" t="s">
         <v>7589</v>
       </c>
       <c r="B72" s="41" t="s">
@@ -26844,13 +26845,13 @@
       <c r="D72" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E72" s="52" t="s">
+      <c r="E72" s="49" t="s">
         <v>7674</v>
       </c>
       <c r="F72" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G72" s="21" t="s">
+      <c r="G72" s="55" t="s">
         <v>7754</v>
       </c>
       <c r="H72" s="18"/>
@@ -26870,7 +26871,7 @@
       <c r="M72" s="21"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A73" s="52" t="s">
+      <c r="A73" s="49" t="s">
         <v>7590</v>
       </c>
       <c r="B73" s="41" t="s">
@@ -26882,13 +26883,13 @@
       <c r="D73" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E73" s="52" t="s">
+      <c r="E73" s="49" t="s">
         <v>7675</v>
       </c>
       <c r="F73" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G73" s="21" t="s">
+      <c r="G73" s="55" t="s">
         <v>7755</v>
       </c>
       <c r="H73" s="18"/>
@@ -26908,7 +26909,7 @@
       <c r="M73" s="21"/>
     </row>
     <row r="74" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A74" s="52" t="s">
+      <c r="A74" s="49" t="s">
         <v>7591</v>
       </c>
       <c r="B74" s="41" t="s">
@@ -26920,13 +26921,13 @@
       <c r="D74" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E74" s="52" t="s">
+      <c r="E74" s="49" t="s">
         <v>7676</v>
       </c>
       <c r="F74" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G74" s="21" t="s">
+      <c r="G74" s="55" t="s">
         <v>7756</v>
       </c>
       <c r="H74" s="18"/>
@@ -26946,7 +26947,7 @@
       <c r="M74" s="21"/>
     </row>
     <row r="75" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A75" s="52" t="s">
+      <c r="A75" s="49" t="s">
         <v>7592</v>
       </c>
       <c r="B75" s="41" t="s">
@@ -26958,13 +26959,13 @@
       <c r="D75" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E75" s="52" t="s">
+      <c r="E75" s="49" t="s">
         <v>7677</v>
       </c>
       <c r="F75" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G75" s="21" t="s">
+      <c r="G75" s="55" t="s">
         <v>7757</v>
       </c>
       <c r="H75" s="18"/>
@@ -26984,7 +26985,7 @@
       <c r="M75" s="21"/>
     </row>
     <row r="76" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A76" s="52" t="s">
+      <c r="A76" s="49" t="s">
         <v>7593</v>
       </c>
       <c r="B76" s="41" t="s">
@@ -26996,13 +26997,13 @@
       <c r="D76" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E76" s="52" t="s">
+      <c r="E76" s="49" t="s">
         <v>7678</v>
       </c>
       <c r="F76" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G76" s="21" t="s">
+      <c r="G76" s="55" t="s">
         <v>7758</v>
       </c>
       <c r="H76" s="18"/>
@@ -27022,7 +27023,7 @@
       <c r="M76" s="21"/>
     </row>
     <row r="77" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A77" s="52" t="s">
+      <c r="A77" s="49" t="s">
         <v>7594</v>
       </c>
       <c r="B77" s="41" t="s">
@@ -27034,13 +27035,13 @@
       <c r="D77" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E77" s="52" t="s">
+      <c r="E77" s="49" t="s">
         <v>7679</v>
       </c>
       <c r="F77" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G77" s="21" t="s">
+      <c r="G77" s="55" t="s">
         <v>7759</v>
       </c>
       <c r="H77" s="18"/>
@@ -27060,7 +27061,7 @@
       <c r="M77" s="21"/>
     </row>
     <row r="78" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A78" s="52" t="s">
+      <c r="A78" s="49" t="s">
         <v>7595</v>
       </c>
       <c r="B78" s="41" t="s">
@@ -27072,13 +27073,13 @@
       <c r="D78" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E78" s="52" t="s">
+      <c r="E78" s="49" t="s">
         <v>7680</v>
       </c>
       <c r="F78" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G78" s="21" t="s">
+      <c r="G78" s="55" t="s">
         <v>7760</v>
       </c>
       <c r="H78" s="18"/>
@@ -27098,7 +27099,7 @@
       <c r="M78" s="21"/>
     </row>
     <row r="79" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A79" s="52" t="s">
+      <c r="A79" s="49" t="s">
         <v>7596</v>
       </c>
       <c r="B79" s="41" t="s">
@@ -27110,13 +27111,13 @@
       <c r="D79" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E79" s="52" t="s">
+      <c r="E79" s="49" t="s">
         <v>7681</v>
       </c>
       <c r="F79" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G79" s="21" t="s">
+      <c r="G79" s="55" t="s">
         <v>7761</v>
       </c>
       <c r="H79" s="18"/>
@@ -27136,7 +27137,7 @@
       <c r="M79" s="21"/>
     </row>
     <row r="80" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A80" s="52" t="s">
+      <c r="A80" s="49" t="s">
         <v>7597</v>
       </c>
       <c r="B80" s="41" t="s">
@@ -27148,13 +27149,13 @@
       <c r="D80" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E80" s="52" t="s">
+      <c r="E80" s="49" t="s">
         <v>7682</v>
       </c>
       <c r="F80" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G80" s="21" t="s">
+      <c r="G80" s="55" t="s">
         <v>7762</v>
       </c>
       <c r="H80" s="18"/>
@@ -27174,7 +27175,7 @@
       <c r="M80" s="21"/>
     </row>
     <row r="81" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A81" s="52" t="s">
+      <c r="A81" s="49" t="s">
         <v>7598</v>
       </c>
       <c r="B81" s="41" t="s">
@@ -27186,13 +27187,13 @@
       <c r="D81" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E81" s="52" t="s">
+      <c r="E81" s="49" t="s">
         <v>7683</v>
       </c>
       <c r="F81" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G81" s="21" t="s">
+      <c r="G81" s="55" t="s">
         <v>7763</v>
       </c>
       <c r="H81" s="18"/>
@@ -27212,7 +27213,7 @@
       <c r="M81" s="21"/>
     </row>
     <row r="82" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A82" s="52" t="s">
+      <c r="A82" s="49" t="s">
         <v>7599</v>
       </c>
       <c r="B82" s="41" t="s">
@@ -27224,13 +27225,13 @@
       <c r="D82" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E82" s="52" t="s">
+      <c r="E82" s="49" t="s">
         <v>7684</v>
       </c>
       <c r="F82" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G82" s="21" t="s">
+      <c r="G82" s="55" t="s">
         <v>7764</v>
       </c>
       <c r="H82" s="18"/>
@@ -27250,7 +27251,7 @@
       <c r="M82" s="21"/>
     </row>
     <row r="83" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A83" s="52" t="s">
+      <c r="A83" s="49" t="s">
         <v>7600</v>
       </c>
       <c r="B83" s="41" t="s">
@@ -27262,13 +27263,13 @@
       <c r="D83" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E83" s="52" t="s">
+      <c r="E83" s="49" t="s">
         <v>7685</v>
       </c>
       <c r="F83" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G83" s="21" t="s">
+      <c r="G83" s="55" t="s">
         <v>7765</v>
       </c>
       <c r="H83" s="18"/>
@@ -27288,7 +27289,7 @@
       <c r="M83" s="21"/>
     </row>
     <row r="84" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A84" s="52" t="s">
+      <c r="A84" s="49" t="s">
         <v>7601</v>
       </c>
       <c r="B84" s="41" t="s">
@@ -27300,13 +27301,13 @@
       <c r="D84" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E84" s="52" t="s">
+      <c r="E84" s="49" t="s">
         <v>7601</v>
       </c>
       <c r="F84" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G84" s="21" t="s">
+      <c r="G84" s="55" t="s">
         <v>7766</v>
       </c>
       <c r="H84" s="18"/>
@@ -27326,7 +27327,7 @@
       <c r="M84" s="21"/>
     </row>
     <row r="85" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A85" s="52" t="s">
+      <c r="A85" s="49" t="s">
         <v>7602</v>
       </c>
       <c r="B85" s="41" t="s">
@@ -27338,13 +27339,13 @@
       <c r="D85" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E85" s="52" t="s">
+      <c r="E85" s="49" t="s">
         <v>7686</v>
       </c>
       <c r="F85" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G85" s="21" t="s">
+      <c r="G85" s="55" t="s">
         <v>7767</v>
       </c>
       <c r="H85" s="18"/>
@@ -27364,7 +27365,7 @@
       <c r="M85" s="21"/>
     </row>
     <row r="86" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A86" s="52" t="s">
+      <c r="A86" s="49" t="s">
         <v>7603</v>
       </c>
       <c r="B86" s="41" t="s">
@@ -27376,13 +27377,13 @@
       <c r="D86" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E86" s="52" t="s">
+      <c r="E86" s="49" t="s">
         <v>7687</v>
       </c>
       <c r="F86" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G86" s="21" t="s">
+      <c r="G86" s="55" t="s">
         <v>7768</v>
       </c>
       <c r="H86" s="18"/>
@@ -27402,7 +27403,7 @@
       <c r="M86" s="21"/>
     </row>
     <row r="87" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A87" s="52" t="s">
+      <c r="A87" s="49" t="s">
         <v>7604</v>
       </c>
       <c r="B87" s="41" t="s">
@@ -27414,13 +27415,13 @@
       <c r="D87" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E87" s="52" t="s">
+      <c r="E87" s="49" t="s">
         <v>7688</v>
       </c>
       <c r="F87" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G87" s="21" t="s">
+      <c r="G87" s="55" t="s">
         <v>7769</v>
       </c>
       <c r="H87" s="18"/>
@@ -27440,7 +27441,7 @@
       <c r="M87" s="21"/>
     </row>
     <row r="88" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A88" s="52" t="s">
+      <c r="A88" s="49" t="s">
         <v>7605</v>
       </c>
       <c r="B88" s="41" t="s">
@@ -27452,13 +27453,13 @@
       <c r="D88" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E88" s="52" t="s">
+      <c r="E88" s="49" t="s">
         <v>7689</v>
       </c>
       <c r="F88" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G88" s="21" t="s">
+      <c r="G88" s="55" t="s">
         <v>7770</v>
       </c>
       <c r="H88" s="18"/>
@@ -27478,7 +27479,7 @@
       <c r="M88" s="21"/>
     </row>
     <row r="89" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A89" s="52" t="s">
+      <c r="A89" s="49" t="s">
         <v>7606</v>
       </c>
       <c r="B89" s="41" t="s">
@@ -27490,13 +27491,13 @@
       <c r="D89" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E89" s="52" t="s">
+      <c r="E89" s="49" t="s">
         <v>7690</v>
       </c>
       <c r="F89" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G89" s="21" t="s">
+      <c r="G89" s="55" t="s">
         <v>7771</v>
       </c>
       <c r="H89" s="18"/>
@@ -27516,7 +27517,7 @@
       <c r="M89" s="21"/>
     </row>
     <row r="90" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A90" s="52" t="s">
+      <c r="A90" s="49" t="s">
         <v>7607</v>
       </c>
       <c r="B90" s="41" t="s">
@@ -27528,13 +27529,13 @@
       <c r="D90" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E90" s="52" t="s">
+      <c r="E90" s="49" t="s">
         <v>7691</v>
       </c>
       <c r="F90" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G90" s="21" t="s">
+      <c r="G90" s="55" t="s">
         <v>7772</v>
       </c>
       <c r="H90" s="18"/>
@@ -27554,7 +27555,7 @@
       <c r="M90" s="21"/>
     </row>
     <row r="91" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A91" s="52" t="s">
+      <c r="A91" s="49" t="s">
         <v>7608</v>
       </c>
       <c r="B91" s="41" t="s">
@@ -27566,13 +27567,13 @@
       <c r="D91" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E91" s="52" t="s">
+      <c r="E91" s="49" t="s">
         <v>7692</v>
       </c>
       <c r="F91" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G91" s="21" t="s">
+      <c r="G91" s="55" t="s">
         <v>7773</v>
       </c>
       <c r="H91" s="18"/>
@@ -27592,7 +27593,7 @@
       <c r="M91" s="21"/>
     </row>
     <row r="92" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A92" s="52" t="s">
+      <c r="A92" s="49" t="s">
         <v>7609</v>
       </c>
       <c r="B92" s="41" t="s">
@@ -27604,13 +27605,13 @@
       <c r="D92" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E92" s="52" t="s">
+      <c r="E92" s="49" t="s">
         <v>7609</v>
       </c>
       <c r="F92" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G92" s="21" t="s">
+      <c r="G92" s="55" t="s">
         <v>7774</v>
       </c>
       <c r="H92" s="18"/>
@@ -27630,7 +27631,7 @@
       <c r="M92" s="21"/>
     </row>
     <row r="93" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A93" s="52" t="s">
+      <c r="A93" s="49" t="s">
         <v>7610</v>
       </c>
       <c r="B93" s="41" t="s">
@@ -27642,13 +27643,13 @@
       <c r="D93" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E93" s="52" t="s">
+      <c r="E93" s="49" t="s">
         <v>7693</v>
       </c>
       <c r="F93" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G93" s="21" t="s">
+      <c r="G93" s="55" t="s">
         <v>7775</v>
       </c>
       <c r="H93" s="18"/>
@@ -27668,7 +27669,7 @@
       <c r="M93" s="21"/>
     </row>
     <row r="94" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A94" s="52" t="s">
+      <c r="A94" s="49" t="s">
         <v>7611</v>
       </c>
       <c r="B94" s="41" t="s">
@@ -27680,13 +27681,13 @@
       <c r="D94" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E94" s="52" t="s">
+      <c r="E94" s="49" t="s">
         <v>7694</v>
       </c>
       <c r="F94" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G94" s="21" t="s">
+      <c r="G94" s="55" t="s">
         <v>7776</v>
       </c>
       <c r="H94" s="18"/>
@@ -27706,7 +27707,7 @@
       <c r="M94" s="21"/>
     </row>
     <row r="95" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A95" s="52" t="s">
+      <c r="A95" s="49" t="s">
         <v>7612</v>
       </c>
       <c r="B95" s="41" t="s">
@@ -27718,13 +27719,13 @@
       <c r="D95" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E95" s="52" t="s">
+      <c r="E95" s="49" t="s">
         <v>7695</v>
       </c>
       <c r="F95" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G95" s="21" t="s">
+      <c r="G95" s="55" t="s">
         <v>7777</v>
       </c>
       <c r="H95" s="18"/>
@@ -27744,7 +27745,7 @@
       <c r="M95" s="21"/>
     </row>
     <row r="96" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A96" s="52" t="s">
+      <c r="A96" s="49" t="s">
         <v>7613</v>
       </c>
       <c r="B96" s="41" t="s">
@@ -27756,13 +27757,13 @@
       <c r="D96" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E96" s="52" t="s">
+      <c r="E96" s="49" t="s">
         <v>7613</v>
       </c>
       <c r="F96" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G96" s="21" t="s">
+      <c r="G96" s="55" t="s">
         <v>7778</v>
       </c>
       <c r="H96" s="18"/>
@@ -27782,7 +27783,7 @@
       <c r="M96" s="21"/>
     </row>
     <row r="97" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A97" s="52" t="s">
+      <c r="A97" s="49" t="s">
         <v>7614</v>
       </c>
       <c r="B97" s="41" t="s">
@@ -27794,13 +27795,13 @@
       <c r="D97" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E97" s="52" t="s">
+      <c r="E97" s="49" t="s">
         <v>7614</v>
       </c>
       <c r="F97" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G97" s="21" t="s">
+      <c r="G97" s="55" t="s">
         <v>7779</v>
       </c>
       <c r="H97" s="18"/>
@@ -27820,7 +27821,7 @@
       <c r="M97" s="21"/>
     </row>
     <row r="98" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A98" s="52" t="s">
+      <c r="A98" s="49" t="s">
         <v>7615</v>
       </c>
       <c r="B98" s="41" t="s">
@@ -27832,13 +27833,13 @@
       <c r="D98" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E98" s="52" t="s">
+      <c r="E98" s="49" t="s">
         <v>7615</v>
       </c>
       <c r="F98" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G98" s="21" t="s">
+      <c r="G98" s="55" t="s">
         <v>7780</v>
       </c>
       <c r="H98" s="18"/>
@@ -28956,10 +28957,96 @@
   <mergeCells count="1">
     <mergeCell ref="A5:F5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G15" r:id="rId1" xr:uid="{91F71076-0402-9149-963B-EAF677C1DFDF}"/>
+    <hyperlink ref="G16" r:id="rId2" xr:uid="{C9E5FFDA-9C2D-0F43-A877-1C7F4FF06051}"/>
+    <hyperlink ref="G17" r:id="rId3" xr:uid="{554DEDC6-BFF9-9743-A774-8A26EFC4DD86}"/>
+    <hyperlink ref="G18" r:id="rId4" xr:uid="{1F92A6E2-C2C3-EF44-A63E-23C01BFC3831}"/>
+    <hyperlink ref="G19" r:id="rId5" xr:uid="{40C63DAE-82C4-0A46-BC7A-ECF0585A8034}"/>
+    <hyperlink ref="G20" r:id="rId6" xr:uid="{3A1A64A2-D2E1-6A42-8843-EA13691A71C9}"/>
+    <hyperlink ref="G21" r:id="rId7" xr:uid="{1A538EAB-27C2-6640-B4EB-7A30DC8DF79C}"/>
+    <hyperlink ref="G22" r:id="rId8" xr:uid="{2275F7F5-D5B8-6249-96FF-41CB66580C46}"/>
+    <hyperlink ref="G23" r:id="rId9" xr:uid="{C5510779-A83D-F04A-97B6-4BCEAE678651}"/>
+    <hyperlink ref="G24" r:id="rId10" xr:uid="{CB06DF4E-5378-FF46-AE4D-F27EB0D4DC79}"/>
+    <hyperlink ref="G25" r:id="rId11" xr:uid="{412F8F0F-16D8-C94D-B175-E039D6097A96}"/>
+    <hyperlink ref="G26" r:id="rId12" xr:uid="{7F738A30-BAB5-304C-A3DB-CD40C97A9777}"/>
+    <hyperlink ref="G27" r:id="rId13" xr:uid="{5E3A9AE3-2897-D14F-AB1E-750080D73331}"/>
+    <hyperlink ref="G28" r:id="rId14" xr:uid="{EDFF1219-1C48-8145-858A-7095A1EFFAFF}"/>
+    <hyperlink ref="G29" r:id="rId15" xr:uid="{66B40662-CA29-1D43-9AB6-1D2D84CB375A}"/>
+    <hyperlink ref="G30" r:id="rId16" xr:uid="{576C341F-D6B1-744C-983D-3CF617A4E48A}"/>
+    <hyperlink ref="G31" r:id="rId17" xr:uid="{418787FE-2905-BB42-8166-FCED518088C6}"/>
+    <hyperlink ref="G32" r:id="rId18" xr:uid="{9C13A40C-258F-DA42-AFC6-5C9BEC802158}"/>
+    <hyperlink ref="G33" r:id="rId19" xr:uid="{79623595-A177-3F49-ADE6-51CC51224B6B}"/>
+    <hyperlink ref="G34" r:id="rId20" xr:uid="{216219A9-70EA-5C4D-B908-BEB7DF7C6EB8}"/>
+    <hyperlink ref="G35" r:id="rId21" xr:uid="{610FDEFB-5F19-104B-8BAB-91BB3DC1195D}"/>
+    <hyperlink ref="G36" r:id="rId22" xr:uid="{DB39E56E-CF9C-9645-8776-1F7DE809462F}"/>
+    <hyperlink ref="G37" r:id="rId23" xr:uid="{6A004C37-665B-224F-B80E-A3AA98ECB006}"/>
+    <hyperlink ref="G38" r:id="rId24" xr:uid="{0FFD22CC-F0BE-1A48-AB35-D554B8D5808A}"/>
+    <hyperlink ref="G39" r:id="rId25" xr:uid="{288B90C6-B28A-6346-A2DA-E8C6276A145C}"/>
+    <hyperlink ref="G40" r:id="rId26" xr:uid="{54175AFA-F34F-8F4A-8326-CED7BE8A9B58}"/>
+    <hyperlink ref="G41" r:id="rId27" xr:uid="{B93CE6DE-D4EC-4D40-A544-D0EE9E085D3C}"/>
+    <hyperlink ref="G42" r:id="rId28" xr:uid="{12C4127B-E0A6-224D-9CC3-E59734536B3D}"/>
+    <hyperlink ref="G43" r:id="rId29" xr:uid="{F6117F5C-A6FE-B54C-9195-763077CA660D}"/>
+    <hyperlink ref="G44" r:id="rId30" xr:uid="{2155CB35-1E56-4246-A3D3-1340939EDE61}"/>
+    <hyperlink ref="G45" r:id="rId31" xr:uid="{ACD1FEBE-91A3-5D4D-95C8-E4824641DDEE}"/>
+    <hyperlink ref="G46" r:id="rId32" xr:uid="{F7D0E799-64CB-F442-95C3-12BDB32E2EE2}"/>
+    <hyperlink ref="G47" r:id="rId33" xr:uid="{4BC43BB8-2B6B-304F-BB05-37F9B14BC936}"/>
+    <hyperlink ref="G48" r:id="rId34" xr:uid="{F1780317-277D-7E4F-8DB3-9C0FE877D378}"/>
+    <hyperlink ref="G49" r:id="rId35" xr:uid="{96953C23-7E19-8749-9A4A-6F41C7227BD4}"/>
+    <hyperlink ref="G50" r:id="rId36" xr:uid="{0D414653-3576-DF4A-BCAE-6C26FFD98384}"/>
+    <hyperlink ref="G51" r:id="rId37" xr:uid="{0BC32026-8765-0C40-B42F-D94897B8B866}"/>
+    <hyperlink ref="G52" r:id="rId38" xr:uid="{24B85AD3-5B76-FD45-93C4-5EF84A443065}"/>
+    <hyperlink ref="G53" r:id="rId39" xr:uid="{55E52E80-EBB2-714C-AB91-588E602BCB07}"/>
+    <hyperlink ref="G54" r:id="rId40" xr:uid="{29A9EFE8-C8CA-A443-B239-50C05D3856A1}"/>
+    <hyperlink ref="G55" r:id="rId41" xr:uid="{F2773AA3-E483-224D-8097-264C76D3C108}"/>
+    <hyperlink ref="G56" r:id="rId42" xr:uid="{C157C614-C5F0-CF4E-B7A3-D32FA6D635A6}"/>
+    <hyperlink ref="G57" r:id="rId43" xr:uid="{ABC98F35-52B7-4C4A-9F37-AC2622D7993F}"/>
+    <hyperlink ref="G58" r:id="rId44" xr:uid="{0C0F3961-5D11-934C-972F-E6323363CEE2}"/>
+    <hyperlink ref="G59" r:id="rId45" xr:uid="{B6A8DC2D-B6B4-0A4E-9AAC-63B6E653A698}"/>
+    <hyperlink ref="G60" r:id="rId46" xr:uid="{86131C4D-BDA9-294E-AC54-6BB2F81A6DA1}"/>
+    <hyperlink ref="G61" r:id="rId47" xr:uid="{E0E47C98-93B8-304E-B967-AD1D8006B163}"/>
+    <hyperlink ref="G62" r:id="rId48" xr:uid="{09A3A2B5-E7E6-E042-B0F1-F6CA0B3C821D}"/>
+    <hyperlink ref="G63" r:id="rId49" xr:uid="{FF19073E-13DB-9542-9BFE-F22B58E72925}"/>
+    <hyperlink ref="G64" r:id="rId50" xr:uid="{47DB1D09-94F7-2C4C-A0B5-943F2137FB16}"/>
+    <hyperlink ref="G65" r:id="rId51" xr:uid="{45458370-9DDD-8244-861A-D9D32776E980}"/>
+    <hyperlink ref="G66" r:id="rId52" xr:uid="{CEDE1A24-148F-AF49-B4EF-F9C6CDAD888B}"/>
+    <hyperlink ref="G67" r:id="rId53" xr:uid="{C08EA231-8D89-FE45-AA9B-431D57982EA3}"/>
+    <hyperlink ref="G68" r:id="rId54" xr:uid="{330BAC4B-A16C-964C-BCEC-EB023690D263}"/>
+    <hyperlink ref="G69" r:id="rId55" xr:uid="{14869655-5125-4043-8BDD-E37C7948C8AB}"/>
+    <hyperlink ref="G70" r:id="rId56" xr:uid="{3CC2888B-1C5A-EE47-BEB6-284A32602E16}"/>
+    <hyperlink ref="G71" r:id="rId57" xr:uid="{31753E4A-5DD2-8A43-A4CF-68208301C82C}"/>
+    <hyperlink ref="G72" r:id="rId58" xr:uid="{55C8EAC8-22DB-704A-88E5-316F74F4EA47}"/>
+    <hyperlink ref="G73" r:id="rId59" xr:uid="{BEACB342-4D88-9C47-B644-040BCF92F1CF}"/>
+    <hyperlink ref="G74" r:id="rId60" xr:uid="{887F9C36-A8EB-C145-A227-286C8FFB4F5D}"/>
+    <hyperlink ref="G75" r:id="rId61" xr:uid="{B0524093-3EA6-0649-9D2E-4852A451A8E5}"/>
+    <hyperlink ref="G76" r:id="rId62" xr:uid="{D82E180F-026E-CA4D-B42F-1C2FA309AB41}"/>
+    <hyperlink ref="G77" r:id="rId63" xr:uid="{AC11962B-84E5-3249-B1EF-C82BDBBCCE16}"/>
+    <hyperlink ref="G78" r:id="rId64" xr:uid="{B07269F3-3D20-1E42-914A-A88FC2187C96}"/>
+    <hyperlink ref="G79" r:id="rId65" xr:uid="{2A6D0C25-29BD-0944-9F31-34C52A89122A}"/>
+    <hyperlink ref="G80" r:id="rId66" xr:uid="{F82D189B-BF6F-CD40-8537-69140D9EC18C}"/>
+    <hyperlink ref="G81" r:id="rId67" xr:uid="{813C4F81-176E-6741-A460-6FC9C63D653C}"/>
+    <hyperlink ref="G82" r:id="rId68" xr:uid="{801CF54B-98C2-F945-AD56-D1049B410FE5}"/>
+    <hyperlink ref="G83" r:id="rId69" xr:uid="{303F6042-EBE4-194A-A291-A8E0FB5EA817}"/>
+    <hyperlink ref="G84" r:id="rId70" xr:uid="{D9FA3B17-B1DE-C649-B2A8-9F82A65D063F}"/>
+    <hyperlink ref="G85" r:id="rId71" xr:uid="{6084F5D4-AE37-D643-8EC9-C768D8A2CED8}"/>
+    <hyperlink ref="G86" r:id="rId72" xr:uid="{2919E0DD-5265-D644-93C0-40611AC2B5FE}"/>
+    <hyperlink ref="G87" r:id="rId73" xr:uid="{D9CE6B37-FD94-604D-967F-DA8F4A3A3D58}"/>
+    <hyperlink ref="G88" r:id="rId74" xr:uid="{C580E03C-217C-2E45-9195-7E5FF61F5307}"/>
+    <hyperlink ref="G89" r:id="rId75" xr:uid="{15C2E4BF-1962-4E49-A483-1781DDFEA0D2}"/>
+    <hyperlink ref="G90" r:id="rId76" xr:uid="{FD88012B-861C-D949-915A-4EB45ECBA112}"/>
+    <hyperlink ref="G91" r:id="rId77" xr:uid="{AA77869A-3223-7F44-B358-1D64C4798AAA}"/>
+    <hyperlink ref="G92" r:id="rId78" xr:uid="{3C5FABFE-EF99-2748-9F8A-3AE181F40722}"/>
+    <hyperlink ref="G93" r:id="rId79" xr:uid="{182169C3-34ED-6644-AD8D-026D0175349A}"/>
+    <hyperlink ref="G94" r:id="rId80" xr:uid="{CC08E01A-F5D6-4441-9660-0770844DAD79}"/>
+    <hyperlink ref="G95" r:id="rId81" xr:uid="{2FB5E4AD-8DCD-1440-BB30-3D1083AC72E6}"/>
+    <hyperlink ref="G96" r:id="rId82" xr:uid="{4D1242ED-DC29-0847-BF8D-B435FFBB8DD6}"/>
+    <hyperlink ref="G97" r:id="rId83" xr:uid="{C10EFD59-A0AB-F146-96D6-449BE233AF4C}"/>
+    <hyperlink ref="G98" r:id="rId84" xr:uid="{AE09611B-1C69-9048-B398-01DD25262534}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId85"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
- downloaded all gb files from FreeGenes into directory - changed xlsx from URL to Local for source - have not updated .gb files to remove issues yet
</commit_message>
<xml_diff>
--- a/Open Enzymes Collection/Open Enzymes Collection.xlsx
+++ b/Open Enzymes Collection/Open Enzymes Collection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Open Enzymes Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDCF4C7-E278-F34C-A185-8EA1857B25FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A9DDE-52F4-0647-9E65-A353F5C311E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23224,256 +23224,256 @@
     <t>Taken from Open Ezymes Collection at FreeGenes</t>
   </si>
   <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003247.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003248.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003249.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003250.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003251.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003252.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003253.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003254.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003255.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003256.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003257.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003258.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003259.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003260.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003261.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003262.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003263.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003264.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003265.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003266.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003267.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003268.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003269.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003270.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003271.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003272.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003273.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003274.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003275.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003276.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003277.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003278.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003279.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003280.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003281.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003282.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003283.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003284.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003285.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003286.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003287.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003288.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003289.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003290.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003291.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003292.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003293.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003294.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003295.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003296.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003297.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003298.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003299.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003300.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003301.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003302.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003303.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003304.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003305.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003306.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003307.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003308.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003309.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003310.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003311.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003312.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003313.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003314.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003315.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003316.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003317.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003318.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003319.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003320.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003321.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003322.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003323.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003324.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003325.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003326.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003327.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003328.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003329.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003330.gb</t>
+    <t>BBF10K_003247.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003248.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003249.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003250.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003251.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003252.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003253.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003254.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003255.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003256.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003257.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003258.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003259.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003260.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003261.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003262.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003263.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003264.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003265.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003266.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003267.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003268.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003269.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003270.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003271.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003272.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003273.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003274.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003275.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003276.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003277.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003278.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003279.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003280.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003281.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003282.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003283.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003284.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003285.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003286.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003287.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003288.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003289.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003290.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003291.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003292.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003293.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003294.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003295.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003296.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003297.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003298.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003299.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003300.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003301.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003302.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003303.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003304.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003305.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003306.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003307.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003308.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003309.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003310.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003311.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003312.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003313.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003314.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003315.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003316.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003317.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003318.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003319.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003320.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003321.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003322.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003323.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003324.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003325.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003326.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003327.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003328.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003329.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003330.gb</t>
   </si>
 </sst>
 </file>
@@ -23824,7 +23824,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23888,7 +23888,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -24340,8 +24339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:G98"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D97" sqref="D25:D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24352,7 +24351,7 @@
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="57.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
     <col min="10" max="11" width="8.42578125" customWidth="1"/>
@@ -24683,9 +24682,9 @@
         <v>7619</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G15" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G15" t="s">
         <v>7697</v>
       </c>
       <c r="H15" s="18"/>
@@ -24721,9 +24720,9 @@
         <v>7620</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G16" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G16" t="s">
         <v>7698</v>
       </c>
       <c r="H16" s="18"/>
@@ -24759,9 +24758,9 @@
         <v>7621</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G17" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G17" t="s">
         <v>7699</v>
       </c>
       <c r="H17" s="18"/>
@@ -24797,9 +24796,9 @@
         <v>7622</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G18" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G18" t="s">
         <v>7700</v>
       </c>
       <c r="H18" s="18"/>
@@ -24835,9 +24834,9 @@
         <v>7623</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G19" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G19" t="s">
         <v>7701</v>
       </c>
       <c r="H19" s="18"/>
@@ -24873,9 +24872,9 @@
         <v>7624</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G20" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G20" t="s">
         <v>7702</v>
       </c>
       <c r="H20" s="18"/>
@@ -24911,9 +24910,9 @@
         <v>7625</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G21" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G21" t="s">
         <v>7703</v>
       </c>
       <c r="H21" s="18"/>
@@ -24949,9 +24948,9 @@
         <v>7626</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G22" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G22" t="s">
         <v>7704</v>
       </c>
       <c r="H22" s="18"/>
@@ -24987,9 +24986,9 @@
         <v>7627</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G23" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G23" t="s">
         <v>7705</v>
       </c>
       <c r="H23" s="18"/>
@@ -25025,9 +25024,9 @@
         <v>7628</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G24" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G24" t="s">
         <v>7706</v>
       </c>
       <c r="H24" s="18"/>
@@ -25063,9 +25062,9 @@
         <v>7629</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G25" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G25" t="s">
         <v>7707</v>
       </c>
       <c r="H25" s="18"/>
@@ -25101,9 +25100,9 @@
         <v>7630</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G26" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G26" t="s">
         <v>7708</v>
       </c>
       <c r="H26" s="18"/>
@@ -25139,9 +25138,9 @@
         <v>7631</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G27" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G27" t="s">
         <v>7709</v>
       </c>
       <c r="H27" s="18"/>
@@ -25177,9 +25176,9 @@
         <v>7632</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G28" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G28" t="s">
         <v>7710</v>
       </c>
       <c r="H28" s="18"/>
@@ -25215,9 +25214,9 @@
         <v>7633</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G29" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G29" t="s">
         <v>7711</v>
       </c>
       <c r="H29" s="18"/>
@@ -25253,9 +25252,9 @@
         <v>7634</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G30" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G30" t="s">
         <v>7712</v>
       </c>
       <c r="H30" s="18"/>
@@ -25291,9 +25290,9 @@
         <v>7635</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G31" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G31" t="s">
         <v>7713</v>
       </c>
       <c r="H31" s="18"/>
@@ -25329,9 +25328,9 @@
         <v>7636</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G32" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G32" t="s">
         <v>7714</v>
       </c>
       <c r="H32" s="18"/>
@@ -25367,9 +25366,9 @@
         <v>7637</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G33" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G33" t="s">
         <v>7715</v>
       </c>
       <c r="H33" s="18"/>
@@ -25405,9 +25404,9 @@
         <v>7638</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G34" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G34" t="s">
         <v>7716</v>
       </c>
       <c r="H34" s="18"/>
@@ -25443,9 +25442,9 @@
         <v>7639</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G35" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G35" t="s">
         <v>7717</v>
       </c>
       <c r="H35" s="18"/>
@@ -25481,9 +25480,9 @@
         <v>7640</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G36" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G36" t="s">
         <v>7718</v>
       </c>
       <c r="H36" s="18"/>
@@ -25519,9 +25518,9 @@
         <v>7641</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G37" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G37" t="s">
         <v>7719</v>
       </c>
       <c r="H37" s="18"/>
@@ -25557,9 +25556,9 @@
         <v>7642</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G38" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G38" t="s">
         <v>7720</v>
       </c>
       <c r="H38" s="18"/>
@@ -25595,9 +25594,9 @@
         <v>7643</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G39" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G39" t="s">
         <v>7721</v>
       </c>
       <c r="H39" s="18"/>
@@ -25633,9 +25632,9 @@
         <v>7644</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G40" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G40" t="s">
         <v>7722</v>
       </c>
       <c r="H40" s="18"/>
@@ -25671,9 +25670,9 @@
         <v>7645</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G41" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G41" t="s">
         <v>7723</v>
       </c>
       <c r="H41" s="18"/>
@@ -25709,9 +25708,9 @@
         <v>7646</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G42" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G42" t="s">
         <v>7724</v>
       </c>
       <c r="H42" s="18"/>
@@ -25747,9 +25746,9 @@
         <v>7647</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G43" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G43" t="s">
         <v>7725</v>
       </c>
       <c r="H43" s="18"/>
@@ -25785,9 +25784,9 @@
         <v>7648</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G44" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G44" t="s">
         <v>7726</v>
       </c>
       <c r="H44" s="18"/>
@@ -25823,9 +25822,9 @@
         <v>7649</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G45" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G45" t="s">
         <v>7727</v>
       </c>
       <c r="H45" s="18"/>
@@ -25861,9 +25860,9 @@
         <v>7650</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G46" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G46" t="s">
         <v>7728</v>
       </c>
       <c r="H46" s="18"/>
@@ -25899,9 +25898,9 @@
         <v>7564</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G47" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G47" t="s">
         <v>7729</v>
       </c>
       <c r="H47" s="18"/>
@@ -25937,9 +25936,9 @@
         <v>7565</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G48" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G48" t="s">
         <v>7730</v>
       </c>
       <c r="H48" s="18"/>
@@ -25975,9 +25974,9 @@
         <v>7651</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G49" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G49" t="s">
         <v>7731</v>
       </c>
       <c r="H49" s="18"/>
@@ -26013,9 +26012,9 @@
         <v>7652</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G50" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G50" t="s">
         <v>7732</v>
       </c>
       <c r="H50" s="18"/>
@@ -26051,9 +26050,9 @@
         <v>7653</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G51" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G51" t="s">
         <v>7733</v>
       </c>
       <c r="H51" s="18"/>
@@ -26089,9 +26088,9 @@
         <v>7654</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G52" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G52" t="s">
         <v>7734</v>
       </c>
       <c r="H52" s="18"/>
@@ -26127,9 +26126,9 @@
         <v>7655</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G53" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G53" t="s">
         <v>7735</v>
       </c>
       <c r="H53" s="18"/>
@@ -26165,9 +26164,9 @@
         <v>7656</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G54" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G54" t="s">
         <v>7736</v>
       </c>
       <c r="H54" s="18"/>
@@ -26203,9 +26202,9 @@
         <v>7657</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G55" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G55" t="s">
         <v>7737</v>
       </c>
       <c r="H55" s="18"/>
@@ -26241,9 +26240,9 @@
         <v>7658</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G56" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G56" t="s">
         <v>7738</v>
       </c>
       <c r="H56" s="18"/>
@@ -26279,9 +26278,9 @@
         <v>7659</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G57" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G57" t="s">
         <v>7739</v>
       </c>
       <c r="H57" s="18"/>
@@ -26317,9 +26316,9 @@
         <v>7660</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G58" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G58" t="s">
         <v>7740</v>
       </c>
       <c r="H58" s="18"/>
@@ -26355,9 +26354,9 @@
         <v>7661</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G59" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G59" t="s">
         <v>7741</v>
       </c>
       <c r="H59" s="18"/>
@@ -26393,9 +26392,9 @@
         <v>7662</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G60" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G60" t="s">
         <v>7742</v>
       </c>
       <c r="H60" s="18"/>
@@ -26431,9 +26430,9 @@
         <v>7663</v>
       </c>
       <c r="F61" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G61" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G61" t="s">
         <v>7743</v>
       </c>
       <c r="H61" s="18"/>
@@ -26469,9 +26468,9 @@
         <v>7664</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G62" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G62" t="s">
         <v>7744</v>
       </c>
       <c r="H62" s="18"/>
@@ -26507,9 +26506,9 @@
         <v>7665</v>
       </c>
       <c r="F63" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G63" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G63" t="s">
         <v>7745</v>
       </c>
       <c r="H63" s="18"/>
@@ -26545,9 +26544,9 @@
         <v>7666</v>
       </c>
       <c r="F64" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G64" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G64" t="s">
         <v>7746</v>
       </c>
       <c r="H64" s="18"/>
@@ -26583,9 +26582,9 @@
         <v>7667</v>
       </c>
       <c r="F65" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G65" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G65" t="s">
         <v>7747</v>
       </c>
       <c r="H65" s="18"/>
@@ -26621,9 +26620,9 @@
         <v>7668</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G66" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G66" t="s">
         <v>7748</v>
       </c>
       <c r="H66" s="18"/>
@@ -26659,9 +26658,9 @@
         <v>7669</v>
       </c>
       <c r="F67" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G67" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G67" t="s">
         <v>7749</v>
       </c>
       <c r="H67" s="18"/>
@@ -26697,9 +26696,9 @@
         <v>7670</v>
       </c>
       <c r="F68" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G68" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G68" t="s">
         <v>7750</v>
       </c>
       <c r="H68" s="18"/>
@@ -26735,9 +26734,9 @@
         <v>7671</v>
       </c>
       <c r="F69" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G69" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G69" t="s">
         <v>7751</v>
       </c>
       <c r="H69" s="18"/>
@@ -26773,9 +26772,9 @@
         <v>7672</v>
       </c>
       <c r="F70" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G70" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G70" t="s">
         <v>7752</v>
       </c>
       <c r="H70" s="18"/>
@@ -26811,9 +26810,9 @@
         <v>7673</v>
       </c>
       <c r="F71" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G71" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G71" t="s">
         <v>7753</v>
       </c>
       <c r="H71" s="18"/>
@@ -26849,9 +26848,9 @@
         <v>7674</v>
       </c>
       <c r="F72" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G72" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G72" t="s">
         <v>7754</v>
       </c>
       <c r="H72" s="18"/>
@@ -26887,9 +26886,9 @@
         <v>7675</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G73" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G73" t="s">
         <v>7755</v>
       </c>
       <c r="H73" s="18"/>
@@ -26925,9 +26924,9 @@
         <v>7676</v>
       </c>
       <c r="F74" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G74" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G74" t="s">
         <v>7756</v>
       </c>
       <c r="H74" s="18"/>
@@ -26963,9 +26962,9 @@
         <v>7677</v>
       </c>
       <c r="F75" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G75" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G75" t="s">
         <v>7757</v>
       </c>
       <c r="H75" s="18"/>
@@ -27001,9 +27000,9 @@
         <v>7678</v>
       </c>
       <c r="F76" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G76" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G76" t="s">
         <v>7758</v>
       </c>
       <c r="H76" s="18"/>
@@ -27039,9 +27038,9 @@
         <v>7679</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G77" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G77" t="s">
         <v>7759</v>
       </c>
       <c r="H77" s="18"/>
@@ -27077,9 +27076,9 @@
         <v>7680</v>
       </c>
       <c r="F78" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G78" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G78" t="s">
         <v>7760</v>
       </c>
       <c r="H78" s="18"/>
@@ -27115,9 +27114,9 @@
         <v>7681</v>
       </c>
       <c r="F79" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G79" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G79" t="s">
         <v>7761</v>
       </c>
       <c r="H79" s="18"/>
@@ -27153,9 +27152,9 @@
         <v>7682</v>
       </c>
       <c r="F80" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G80" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G80" t="s">
         <v>7762</v>
       </c>
       <c r="H80" s="18"/>
@@ -27191,9 +27190,9 @@
         <v>7683</v>
       </c>
       <c r="F81" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G81" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G81" t="s">
         <v>7763</v>
       </c>
       <c r="H81" s="18"/>
@@ -27229,9 +27228,9 @@
         <v>7684</v>
       </c>
       <c r="F82" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G82" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G82" t="s">
         <v>7764</v>
       </c>
       <c r="H82" s="18"/>
@@ -27267,9 +27266,9 @@
         <v>7685</v>
       </c>
       <c r="F83" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G83" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G83" t="s">
         <v>7765</v>
       </c>
       <c r="H83" s="18"/>
@@ -27305,9 +27304,9 @@
         <v>7601</v>
       </c>
       <c r="F84" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G84" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G84" t="s">
         <v>7766</v>
       </c>
       <c r="H84" s="18"/>
@@ -27343,9 +27342,9 @@
         <v>7686</v>
       </c>
       <c r="F85" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G85" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G85" t="s">
         <v>7767</v>
       </c>
       <c r="H85" s="18"/>
@@ -27381,9 +27380,9 @@
         <v>7687</v>
       </c>
       <c r="F86" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G86" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G86" t="s">
         <v>7768</v>
       </c>
       <c r="H86" s="18"/>
@@ -27419,9 +27418,9 @@
         <v>7688</v>
       </c>
       <c r="F87" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G87" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G87" t="s">
         <v>7769</v>
       </c>
       <c r="H87" s="18"/>
@@ -27457,9 +27456,9 @@
         <v>7689</v>
       </c>
       <c r="F88" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G88" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G88" t="s">
         <v>7770</v>
       </c>
       <c r="H88" s="18"/>
@@ -27495,9 +27494,9 @@
         <v>7690</v>
       </c>
       <c r="F89" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G89" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G89" t="s">
         <v>7771</v>
       </c>
       <c r="H89" s="18"/>
@@ -27533,9 +27532,9 @@
         <v>7691</v>
       </c>
       <c r="F90" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G90" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G90" t="s">
         <v>7772</v>
       </c>
       <c r="H90" s="18"/>
@@ -27571,9 +27570,9 @@
         <v>7692</v>
       </c>
       <c r="F91" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G91" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G91" t="s">
         <v>7773</v>
       </c>
       <c r="H91" s="18"/>
@@ -27609,9 +27608,9 @@
         <v>7609</v>
       </c>
       <c r="F92" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G92" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G92" t="s">
         <v>7774</v>
       </c>
       <c r="H92" s="18"/>
@@ -27647,9 +27646,9 @@
         <v>7693</v>
       </c>
       <c r="F93" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G93" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G93" t="s">
         <v>7775</v>
       </c>
       <c r="H93" s="18"/>
@@ -27685,9 +27684,9 @@
         <v>7694</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G94" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G94" t="s">
         <v>7776</v>
       </c>
       <c r="H94" s="18"/>
@@ -27723,9 +27722,9 @@
         <v>7695</v>
       </c>
       <c r="F95" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G95" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G95" t="s">
         <v>7777</v>
       </c>
       <c r="H95" s="18"/>
@@ -27761,9 +27760,9 @@
         <v>7613</v>
       </c>
       <c r="F96" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G96" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G96" t="s">
         <v>7778</v>
       </c>
       <c r="H96" s="18"/>
@@ -27799,9 +27798,9 @@
         <v>7614</v>
       </c>
       <c r="F97" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G97" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G97" t="s">
         <v>7779</v>
       </c>
       <c r="H97" s="18"/>
@@ -27837,9 +27836,9 @@
         <v>7615</v>
       </c>
       <c r="F98" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G98" s="55" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G98" t="s">
         <v>7780</v>
       </c>
       <c r="H98" s="18"/>
@@ -28958,90 +28957,90 @@
     <mergeCell ref="A5:F5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G15" r:id="rId1" xr:uid="{91F71076-0402-9149-963B-EAF677C1DFDF}"/>
-    <hyperlink ref="G16" r:id="rId2" xr:uid="{C9E5FFDA-9C2D-0F43-A877-1C7F4FF06051}"/>
-    <hyperlink ref="G17" r:id="rId3" xr:uid="{554DEDC6-BFF9-9743-A774-8A26EFC4DD86}"/>
-    <hyperlink ref="G18" r:id="rId4" xr:uid="{1F92A6E2-C2C3-EF44-A63E-23C01BFC3831}"/>
-    <hyperlink ref="G19" r:id="rId5" xr:uid="{40C63DAE-82C4-0A46-BC7A-ECF0585A8034}"/>
-    <hyperlink ref="G20" r:id="rId6" xr:uid="{3A1A64A2-D2E1-6A42-8843-EA13691A71C9}"/>
-    <hyperlink ref="G21" r:id="rId7" xr:uid="{1A538EAB-27C2-6640-B4EB-7A30DC8DF79C}"/>
-    <hyperlink ref="G22" r:id="rId8" xr:uid="{2275F7F5-D5B8-6249-96FF-41CB66580C46}"/>
-    <hyperlink ref="G23" r:id="rId9" xr:uid="{C5510779-A83D-F04A-97B6-4BCEAE678651}"/>
-    <hyperlink ref="G24" r:id="rId10" xr:uid="{CB06DF4E-5378-FF46-AE4D-F27EB0D4DC79}"/>
-    <hyperlink ref="G25" r:id="rId11" xr:uid="{412F8F0F-16D8-C94D-B175-E039D6097A96}"/>
-    <hyperlink ref="G26" r:id="rId12" xr:uid="{7F738A30-BAB5-304C-A3DB-CD40C97A9777}"/>
-    <hyperlink ref="G27" r:id="rId13" xr:uid="{5E3A9AE3-2897-D14F-AB1E-750080D73331}"/>
-    <hyperlink ref="G28" r:id="rId14" xr:uid="{EDFF1219-1C48-8145-858A-7095A1EFFAFF}"/>
-    <hyperlink ref="G29" r:id="rId15" xr:uid="{66B40662-CA29-1D43-9AB6-1D2D84CB375A}"/>
-    <hyperlink ref="G30" r:id="rId16" xr:uid="{576C341F-D6B1-744C-983D-3CF617A4E48A}"/>
-    <hyperlink ref="G31" r:id="rId17" xr:uid="{418787FE-2905-BB42-8166-FCED518088C6}"/>
-    <hyperlink ref="G32" r:id="rId18" xr:uid="{9C13A40C-258F-DA42-AFC6-5C9BEC802158}"/>
-    <hyperlink ref="G33" r:id="rId19" xr:uid="{79623595-A177-3F49-ADE6-51CC51224B6B}"/>
-    <hyperlink ref="G34" r:id="rId20" xr:uid="{216219A9-70EA-5C4D-B908-BEB7DF7C6EB8}"/>
-    <hyperlink ref="G35" r:id="rId21" xr:uid="{610FDEFB-5F19-104B-8BAB-91BB3DC1195D}"/>
-    <hyperlink ref="G36" r:id="rId22" xr:uid="{DB39E56E-CF9C-9645-8776-1F7DE809462F}"/>
-    <hyperlink ref="G37" r:id="rId23" xr:uid="{6A004C37-665B-224F-B80E-A3AA98ECB006}"/>
-    <hyperlink ref="G38" r:id="rId24" xr:uid="{0FFD22CC-F0BE-1A48-AB35-D554B8D5808A}"/>
-    <hyperlink ref="G39" r:id="rId25" xr:uid="{288B90C6-B28A-6346-A2DA-E8C6276A145C}"/>
-    <hyperlink ref="G40" r:id="rId26" xr:uid="{54175AFA-F34F-8F4A-8326-CED7BE8A9B58}"/>
-    <hyperlink ref="G41" r:id="rId27" xr:uid="{B93CE6DE-D4EC-4D40-A544-D0EE9E085D3C}"/>
-    <hyperlink ref="G42" r:id="rId28" xr:uid="{12C4127B-E0A6-224D-9CC3-E59734536B3D}"/>
-    <hyperlink ref="G43" r:id="rId29" xr:uid="{F6117F5C-A6FE-B54C-9195-763077CA660D}"/>
-    <hyperlink ref="G44" r:id="rId30" xr:uid="{2155CB35-1E56-4246-A3D3-1340939EDE61}"/>
-    <hyperlink ref="G45" r:id="rId31" xr:uid="{ACD1FEBE-91A3-5D4D-95C8-E4824641DDEE}"/>
-    <hyperlink ref="G46" r:id="rId32" xr:uid="{F7D0E799-64CB-F442-95C3-12BDB32E2EE2}"/>
-    <hyperlink ref="G47" r:id="rId33" xr:uid="{4BC43BB8-2B6B-304F-BB05-37F9B14BC936}"/>
-    <hyperlink ref="G48" r:id="rId34" xr:uid="{F1780317-277D-7E4F-8DB3-9C0FE877D378}"/>
-    <hyperlink ref="G49" r:id="rId35" xr:uid="{96953C23-7E19-8749-9A4A-6F41C7227BD4}"/>
-    <hyperlink ref="G50" r:id="rId36" xr:uid="{0D414653-3576-DF4A-BCAE-6C26FFD98384}"/>
-    <hyperlink ref="G51" r:id="rId37" xr:uid="{0BC32026-8765-0C40-B42F-D94897B8B866}"/>
-    <hyperlink ref="G52" r:id="rId38" xr:uid="{24B85AD3-5B76-FD45-93C4-5EF84A443065}"/>
-    <hyperlink ref="G53" r:id="rId39" xr:uid="{55E52E80-EBB2-714C-AB91-588E602BCB07}"/>
-    <hyperlink ref="G54" r:id="rId40" xr:uid="{29A9EFE8-C8CA-A443-B239-50C05D3856A1}"/>
-    <hyperlink ref="G55" r:id="rId41" xr:uid="{F2773AA3-E483-224D-8097-264C76D3C108}"/>
-    <hyperlink ref="G56" r:id="rId42" xr:uid="{C157C614-C5F0-CF4E-B7A3-D32FA6D635A6}"/>
-    <hyperlink ref="G57" r:id="rId43" xr:uid="{ABC98F35-52B7-4C4A-9F37-AC2622D7993F}"/>
-    <hyperlink ref="G58" r:id="rId44" xr:uid="{0C0F3961-5D11-934C-972F-E6323363CEE2}"/>
-    <hyperlink ref="G59" r:id="rId45" xr:uid="{B6A8DC2D-B6B4-0A4E-9AAC-63B6E653A698}"/>
-    <hyperlink ref="G60" r:id="rId46" xr:uid="{86131C4D-BDA9-294E-AC54-6BB2F81A6DA1}"/>
-    <hyperlink ref="G61" r:id="rId47" xr:uid="{E0E47C98-93B8-304E-B967-AD1D8006B163}"/>
-    <hyperlink ref="G62" r:id="rId48" xr:uid="{09A3A2B5-E7E6-E042-B0F1-F6CA0B3C821D}"/>
-    <hyperlink ref="G63" r:id="rId49" xr:uid="{FF19073E-13DB-9542-9BFE-F22B58E72925}"/>
-    <hyperlink ref="G64" r:id="rId50" xr:uid="{47DB1D09-94F7-2C4C-A0B5-943F2137FB16}"/>
-    <hyperlink ref="G65" r:id="rId51" xr:uid="{45458370-9DDD-8244-861A-D9D32776E980}"/>
-    <hyperlink ref="G66" r:id="rId52" xr:uid="{CEDE1A24-148F-AF49-B4EF-F9C6CDAD888B}"/>
-    <hyperlink ref="G67" r:id="rId53" xr:uid="{C08EA231-8D89-FE45-AA9B-431D57982EA3}"/>
-    <hyperlink ref="G68" r:id="rId54" xr:uid="{330BAC4B-A16C-964C-BCEC-EB023690D263}"/>
-    <hyperlink ref="G69" r:id="rId55" xr:uid="{14869655-5125-4043-8BDD-E37C7948C8AB}"/>
-    <hyperlink ref="G70" r:id="rId56" xr:uid="{3CC2888B-1C5A-EE47-BEB6-284A32602E16}"/>
-    <hyperlink ref="G71" r:id="rId57" xr:uid="{31753E4A-5DD2-8A43-A4CF-68208301C82C}"/>
-    <hyperlink ref="G72" r:id="rId58" xr:uid="{55C8EAC8-22DB-704A-88E5-316F74F4EA47}"/>
-    <hyperlink ref="G73" r:id="rId59" xr:uid="{BEACB342-4D88-9C47-B644-040BCF92F1CF}"/>
-    <hyperlink ref="G74" r:id="rId60" xr:uid="{887F9C36-A8EB-C145-A227-286C8FFB4F5D}"/>
-    <hyperlink ref="G75" r:id="rId61" xr:uid="{B0524093-3EA6-0649-9D2E-4852A451A8E5}"/>
-    <hyperlink ref="G76" r:id="rId62" xr:uid="{D82E180F-026E-CA4D-B42F-1C2FA309AB41}"/>
-    <hyperlink ref="G77" r:id="rId63" xr:uid="{AC11962B-84E5-3249-B1EF-C82BDBBCCE16}"/>
-    <hyperlink ref="G78" r:id="rId64" xr:uid="{B07269F3-3D20-1E42-914A-A88FC2187C96}"/>
-    <hyperlink ref="G79" r:id="rId65" xr:uid="{2A6D0C25-29BD-0944-9F31-34C52A89122A}"/>
-    <hyperlink ref="G80" r:id="rId66" xr:uid="{F82D189B-BF6F-CD40-8537-69140D9EC18C}"/>
-    <hyperlink ref="G81" r:id="rId67" xr:uid="{813C4F81-176E-6741-A460-6FC9C63D653C}"/>
-    <hyperlink ref="G82" r:id="rId68" xr:uid="{801CF54B-98C2-F945-AD56-D1049B410FE5}"/>
-    <hyperlink ref="G83" r:id="rId69" xr:uid="{303F6042-EBE4-194A-A291-A8E0FB5EA817}"/>
-    <hyperlink ref="G84" r:id="rId70" xr:uid="{D9FA3B17-B1DE-C649-B2A8-9F82A65D063F}"/>
-    <hyperlink ref="G85" r:id="rId71" xr:uid="{6084F5D4-AE37-D643-8EC9-C768D8A2CED8}"/>
-    <hyperlink ref="G86" r:id="rId72" xr:uid="{2919E0DD-5265-D644-93C0-40611AC2B5FE}"/>
-    <hyperlink ref="G87" r:id="rId73" xr:uid="{D9CE6B37-FD94-604D-967F-DA8F4A3A3D58}"/>
-    <hyperlink ref="G88" r:id="rId74" xr:uid="{C580E03C-217C-2E45-9195-7E5FF61F5307}"/>
-    <hyperlink ref="G89" r:id="rId75" xr:uid="{15C2E4BF-1962-4E49-A483-1781DDFEA0D2}"/>
-    <hyperlink ref="G90" r:id="rId76" xr:uid="{FD88012B-861C-D949-915A-4EB45ECBA112}"/>
-    <hyperlink ref="G91" r:id="rId77" xr:uid="{AA77869A-3223-7F44-B358-1D64C4798AAA}"/>
-    <hyperlink ref="G92" r:id="rId78" xr:uid="{3C5FABFE-EF99-2748-9F8A-3AE181F40722}"/>
-    <hyperlink ref="G93" r:id="rId79" xr:uid="{182169C3-34ED-6644-AD8D-026D0175349A}"/>
-    <hyperlink ref="G94" r:id="rId80" xr:uid="{CC08E01A-F5D6-4441-9660-0770844DAD79}"/>
-    <hyperlink ref="G95" r:id="rId81" xr:uid="{2FB5E4AD-8DCD-1440-BB30-3D1083AC72E6}"/>
-    <hyperlink ref="G96" r:id="rId82" xr:uid="{4D1242ED-DC29-0847-BF8D-B435FFBB8DD6}"/>
-    <hyperlink ref="G97" r:id="rId83" xr:uid="{C10EFD59-A0AB-F146-96D6-449BE233AF4C}"/>
-    <hyperlink ref="G98" r:id="rId84" xr:uid="{AE09611B-1C69-9048-B398-01DD25262534}"/>
+    <hyperlink ref="G15" r:id="rId1" display="https://freegenes.github.io/genbank/BBF10K_003247.gb" xr:uid="{91F71076-0402-9149-963B-EAF677C1DFDF}"/>
+    <hyperlink ref="G16" r:id="rId2" display="https://freegenes.github.io/genbank/BBF10K_003248.gb" xr:uid="{C9E5FFDA-9C2D-0F43-A877-1C7F4FF06051}"/>
+    <hyperlink ref="G17" r:id="rId3" display="https://freegenes.github.io/genbank/BBF10K_003249.gb" xr:uid="{554DEDC6-BFF9-9743-A774-8A26EFC4DD86}"/>
+    <hyperlink ref="G18" r:id="rId4" display="https://freegenes.github.io/genbank/BBF10K_003250.gb" xr:uid="{1F92A6E2-C2C3-EF44-A63E-23C01BFC3831}"/>
+    <hyperlink ref="G19" r:id="rId5" display="https://freegenes.github.io/genbank/BBF10K_003251.gb" xr:uid="{40C63DAE-82C4-0A46-BC7A-ECF0585A8034}"/>
+    <hyperlink ref="G20" r:id="rId6" display="https://freegenes.github.io/genbank/BBF10K_003252.gb" xr:uid="{3A1A64A2-D2E1-6A42-8843-EA13691A71C9}"/>
+    <hyperlink ref="G21" r:id="rId7" display="https://freegenes.github.io/genbank/BBF10K_003253.gb" xr:uid="{1A538EAB-27C2-6640-B4EB-7A30DC8DF79C}"/>
+    <hyperlink ref="G22" r:id="rId8" display="https://freegenes.github.io/genbank/BBF10K_003254.gb" xr:uid="{2275F7F5-D5B8-6249-96FF-41CB66580C46}"/>
+    <hyperlink ref="G23" r:id="rId9" display="https://freegenes.github.io/genbank/BBF10K_003255.gb" xr:uid="{C5510779-A83D-F04A-97B6-4BCEAE678651}"/>
+    <hyperlink ref="G24" r:id="rId10" display="https://freegenes.github.io/genbank/BBF10K_003256.gb" xr:uid="{CB06DF4E-5378-FF46-AE4D-F27EB0D4DC79}"/>
+    <hyperlink ref="G25" r:id="rId11" display="https://freegenes.github.io/genbank/BBF10K_003257.gb" xr:uid="{412F8F0F-16D8-C94D-B175-E039D6097A96}"/>
+    <hyperlink ref="G26" r:id="rId12" display="https://freegenes.github.io/genbank/BBF10K_003258.gb" xr:uid="{7F738A30-BAB5-304C-A3DB-CD40C97A9777}"/>
+    <hyperlink ref="G27" r:id="rId13" display="https://freegenes.github.io/genbank/BBF10K_003259.gb" xr:uid="{5E3A9AE3-2897-D14F-AB1E-750080D73331}"/>
+    <hyperlink ref="G28" r:id="rId14" display="https://freegenes.github.io/genbank/BBF10K_003260.gb" xr:uid="{EDFF1219-1C48-8145-858A-7095A1EFFAFF}"/>
+    <hyperlink ref="G29" r:id="rId15" display="https://freegenes.github.io/genbank/BBF10K_003261.gb" xr:uid="{66B40662-CA29-1D43-9AB6-1D2D84CB375A}"/>
+    <hyperlink ref="G30" r:id="rId16" display="https://freegenes.github.io/genbank/BBF10K_003262.gb" xr:uid="{576C341F-D6B1-744C-983D-3CF617A4E48A}"/>
+    <hyperlink ref="G31" r:id="rId17" display="https://freegenes.github.io/genbank/BBF10K_003263.gb" xr:uid="{418787FE-2905-BB42-8166-FCED518088C6}"/>
+    <hyperlink ref="G32" r:id="rId18" display="https://freegenes.github.io/genbank/BBF10K_003264.gb" xr:uid="{9C13A40C-258F-DA42-AFC6-5C9BEC802158}"/>
+    <hyperlink ref="G33" r:id="rId19" display="https://freegenes.github.io/genbank/BBF10K_003265.gb" xr:uid="{79623595-A177-3F49-ADE6-51CC51224B6B}"/>
+    <hyperlink ref="G34" r:id="rId20" display="https://freegenes.github.io/genbank/BBF10K_003266.gb" xr:uid="{216219A9-70EA-5C4D-B908-BEB7DF7C6EB8}"/>
+    <hyperlink ref="G35" r:id="rId21" display="https://freegenes.github.io/genbank/BBF10K_003267.gb" xr:uid="{610FDEFB-5F19-104B-8BAB-91BB3DC1195D}"/>
+    <hyperlink ref="G36" r:id="rId22" display="https://freegenes.github.io/genbank/BBF10K_003268.gb" xr:uid="{DB39E56E-CF9C-9645-8776-1F7DE809462F}"/>
+    <hyperlink ref="G37" r:id="rId23" display="https://freegenes.github.io/genbank/BBF10K_003269.gb" xr:uid="{6A004C37-665B-224F-B80E-A3AA98ECB006}"/>
+    <hyperlink ref="G38" r:id="rId24" display="https://freegenes.github.io/genbank/BBF10K_003270.gb" xr:uid="{0FFD22CC-F0BE-1A48-AB35-D554B8D5808A}"/>
+    <hyperlink ref="G39" r:id="rId25" display="https://freegenes.github.io/genbank/BBF10K_003271.gb" xr:uid="{288B90C6-B28A-6346-A2DA-E8C6276A145C}"/>
+    <hyperlink ref="G40" r:id="rId26" display="https://freegenes.github.io/genbank/BBF10K_003272.gb" xr:uid="{54175AFA-F34F-8F4A-8326-CED7BE8A9B58}"/>
+    <hyperlink ref="G41" r:id="rId27" display="https://freegenes.github.io/genbank/BBF10K_003273.gb" xr:uid="{B93CE6DE-D4EC-4D40-A544-D0EE9E085D3C}"/>
+    <hyperlink ref="G42" r:id="rId28" display="https://freegenes.github.io/genbank/BBF10K_003274.gb" xr:uid="{12C4127B-E0A6-224D-9CC3-E59734536B3D}"/>
+    <hyperlink ref="G43" r:id="rId29" display="https://freegenes.github.io/genbank/BBF10K_003275.gb" xr:uid="{F6117F5C-A6FE-B54C-9195-763077CA660D}"/>
+    <hyperlink ref="G44" r:id="rId30" display="https://freegenes.github.io/genbank/BBF10K_003276.gb" xr:uid="{2155CB35-1E56-4246-A3D3-1340939EDE61}"/>
+    <hyperlink ref="G45" r:id="rId31" display="https://freegenes.github.io/genbank/BBF10K_003277.gb" xr:uid="{ACD1FEBE-91A3-5D4D-95C8-E4824641DDEE}"/>
+    <hyperlink ref="G46" r:id="rId32" display="https://freegenes.github.io/genbank/BBF10K_003278.gb" xr:uid="{F7D0E799-64CB-F442-95C3-12BDB32E2EE2}"/>
+    <hyperlink ref="G47" r:id="rId33" display="https://freegenes.github.io/genbank/BBF10K_003279.gb" xr:uid="{4BC43BB8-2B6B-304F-BB05-37F9B14BC936}"/>
+    <hyperlink ref="G48" r:id="rId34" display="https://freegenes.github.io/genbank/BBF10K_003280.gb" xr:uid="{F1780317-277D-7E4F-8DB3-9C0FE877D378}"/>
+    <hyperlink ref="G49" r:id="rId35" display="https://freegenes.github.io/genbank/BBF10K_003281.gb" xr:uid="{96953C23-7E19-8749-9A4A-6F41C7227BD4}"/>
+    <hyperlink ref="G50" r:id="rId36" display="https://freegenes.github.io/genbank/BBF10K_003282.gb" xr:uid="{0D414653-3576-DF4A-BCAE-6C26FFD98384}"/>
+    <hyperlink ref="G51" r:id="rId37" display="https://freegenes.github.io/genbank/BBF10K_003283.gb" xr:uid="{0BC32026-8765-0C40-B42F-D94897B8B866}"/>
+    <hyperlink ref="G52" r:id="rId38" display="https://freegenes.github.io/genbank/BBF10K_003284.gb" xr:uid="{24B85AD3-5B76-FD45-93C4-5EF84A443065}"/>
+    <hyperlink ref="G53" r:id="rId39" display="https://freegenes.github.io/genbank/BBF10K_003285.gb" xr:uid="{55E52E80-EBB2-714C-AB91-588E602BCB07}"/>
+    <hyperlink ref="G54" r:id="rId40" display="https://freegenes.github.io/genbank/BBF10K_003286.gb" xr:uid="{29A9EFE8-C8CA-A443-B239-50C05D3856A1}"/>
+    <hyperlink ref="G55" r:id="rId41" display="https://freegenes.github.io/genbank/BBF10K_003287.gb" xr:uid="{F2773AA3-E483-224D-8097-264C76D3C108}"/>
+    <hyperlink ref="G56" r:id="rId42" display="https://freegenes.github.io/genbank/BBF10K_003288.gb" xr:uid="{C157C614-C5F0-CF4E-B7A3-D32FA6D635A6}"/>
+    <hyperlink ref="G57" r:id="rId43" display="https://freegenes.github.io/genbank/BBF10K_003289.gb" xr:uid="{ABC98F35-52B7-4C4A-9F37-AC2622D7993F}"/>
+    <hyperlink ref="G58" r:id="rId44" display="https://freegenes.github.io/genbank/BBF10K_003290.gb" xr:uid="{0C0F3961-5D11-934C-972F-E6323363CEE2}"/>
+    <hyperlink ref="G59" r:id="rId45" display="https://freegenes.github.io/genbank/BBF10K_003291.gb" xr:uid="{B6A8DC2D-B6B4-0A4E-9AAC-63B6E653A698}"/>
+    <hyperlink ref="G60" r:id="rId46" display="https://freegenes.github.io/genbank/BBF10K_003292.gb" xr:uid="{86131C4D-BDA9-294E-AC54-6BB2F81A6DA1}"/>
+    <hyperlink ref="G61" r:id="rId47" display="https://freegenes.github.io/genbank/BBF10K_003293.gb" xr:uid="{E0E47C98-93B8-304E-B967-AD1D8006B163}"/>
+    <hyperlink ref="G62" r:id="rId48" display="https://freegenes.github.io/genbank/BBF10K_003294.gb" xr:uid="{09A3A2B5-E7E6-E042-B0F1-F6CA0B3C821D}"/>
+    <hyperlink ref="G63" r:id="rId49" display="https://freegenes.github.io/genbank/BBF10K_003295.gb" xr:uid="{FF19073E-13DB-9542-9BFE-F22B58E72925}"/>
+    <hyperlink ref="G64" r:id="rId50" display="https://freegenes.github.io/genbank/BBF10K_003296.gb" xr:uid="{47DB1D09-94F7-2C4C-A0B5-943F2137FB16}"/>
+    <hyperlink ref="G65" r:id="rId51" display="https://freegenes.github.io/genbank/BBF10K_003297.gb" xr:uid="{45458370-9DDD-8244-861A-D9D32776E980}"/>
+    <hyperlink ref="G66" r:id="rId52" display="https://freegenes.github.io/genbank/BBF10K_003298.gb" xr:uid="{CEDE1A24-148F-AF49-B4EF-F9C6CDAD888B}"/>
+    <hyperlink ref="G67" r:id="rId53" display="https://freegenes.github.io/genbank/BBF10K_003299.gb" xr:uid="{C08EA231-8D89-FE45-AA9B-431D57982EA3}"/>
+    <hyperlink ref="G68" r:id="rId54" display="https://freegenes.github.io/genbank/BBF10K_003300.gb" xr:uid="{330BAC4B-A16C-964C-BCEC-EB023690D263}"/>
+    <hyperlink ref="G69" r:id="rId55" display="https://freegenes.github.io/genbank/BBF10K_003301.gb" xr:uid="{14869655-5125-4043-8BDD-E37C7948C8AB}"/>
+    <hyperlink ref="G70" r:id="rId56" display="https://freegenes.github.io/genbank/BBF10K_003302.gb" xr:uid="{3CC2888B-1C5A-EE47-BEB6-284A32602E16}"/>
+    <hyperlink ref="G71" r:id="rId57" display="https://freegenes.github.io/genbank/BBF10K_003303.gb" xr:uid="{31753E4A-5DD2-8A43-A4CF-68208301C82C}"/>
+    <hyperlink ref="G72" r:id="rId58" display="https://freegenes.github.io/genbank/BBF10K_003304.gb" xr:uid="{55C8EAC8-22DB-704A-88E5-316F74F4EA47}"/>
+    <hyperlink ref="G73" r:id="rId59" display="https://freegenes.github.io/genbank/BBF10K_003305.gb" xr:uid="{BEACB342-4D88-9C47-B644-040BCF92F1CF}"/>
+    <hyperlink ref="G74" r:id="rId60" display="https://freegenes.github.io/genbank/BBF10K_003306.gb" xr:uid="{887F9C36-A8EB-C145-A227-286C8FFB4F5D}"/>
+    <hyperlink ref="G75" r:id="rId61" display="https://freegenes.github.io/genbank/BBF10K_003307.gb" xr:uid="{B0524093-3EA6-0649-9D2E-4852A451A8E5}"/>
+    <hyperlink ref="G76" r:id="rId62" display="https://freegenes.github.io/genbank/BBF10K_003308.gb" xr:uid="{D82E180F-026E-CA4D-B42F-1C2FA309AB41}"/>
+    <hyperlink ref="G77" r:id="rId63" display="https://freegenes.github.io/genbank/BBF10K_003309.gb" xr:uid="{AC11962B-84E5-3249-B1EF-C82BDBBCCE16}"/>
+    <hyperlink ref="G78" r:id="rId64" display="https://freegenes.github.io/genbank/BBF10K_003310.gb" xr:uid="{B07269F3-3D20-1E42-914A-A88FC2187C96}"/>
+    <hyperlink ref="G79" r:id="rId65" display="https://freegenes.github.io/genbank/BBF10K_003311.gb" xr:uid="{2A6D0C25-29BD-0944-9F31-34C52A89122A}"/>
+    <hyperlink ref="G80" r:id="rId66" display="https://freegenes.github.io/genbank/BBF10K_003312.gb" xr:uid="{F82D189B-BF6F-CD40-8537-69140D9EC18C}"/>
+    <hyperlink ref="G81" r:id="rId67" display="https://freegenes.github.io/genbank/BBF10K_003313.gb" xr:uid="{813C4F81-176E-6741-A460-6FC9C63D653C}"/>
+    <hyperlink ref="G82" r:id="rId68" display="https://freegenes.github.io/genbank/BBF10K_003314.gb" xr:uid="{801CF54B-98C2-F945-AD56-D1049B410FE5}"/>
+    <hyperlink ref="G83" r:id="rId69" display="https://freegenes.github.io/genbank/BBF10K_003315.gb" xr:uid="{303F6042-EBE4-194A-A291-A8E0FB5EA817}"/>
+    <hyperlink ref="G84" r:id="rId70" display="https://freegenes.github.io/genbank/BBF10K_003316.gb" xr:uid="{D9FA3B17-B1DE-C649-B2A8-9F82A65D063F}"/>
+    <hyperlink ref="G85" r:id="rId71" display="https://freegenes.github.io/genbank/BBF10K_003317.gb" xr:uid="{6084F5D4-AE37-D643-8EC9-C768D8A2CED8}"/>
+    <hyperlink ref="G86" r:id="rId72" display="https://freegenes.github.io/genbank/BBF10K_003318.gb" xr:uid="{2919E0DD-5265-D644-93C0-40611AC2B5FE}"/>
+    <hyperlink ref="G87" r:id="rId73" display="https://freegenes.github.io/genbank/BBF10K_003319.gb" xr:uid="{D9CE6B37-FD94-604D-967F-DA8F4A3A3D58}"/>
+    <hyperlink ref="G88" r:id="rId74" display="https://freegenes.github.io/genbank/BBF10K_003320.gb" xr:uid="{C580E03C-217C-2E45-9195-7E5FF61F5307}"/>
+    <hyperlink ref="G89" r:id="rId75" display="https://freegenes.github.io/genbank/BBF10K_003321.gb" xr:uid="{15C2E4BF-1962-4E49-A483-1781DDFEA0D2}"/>
+    <hyperlink ref="G90" r:id="rId76" display="https://freegenes.github.io/genbank/BBF10K_003322.gb" xr:uid="{FD88012B-861C-D949-915A-4EB45ECBA112}"/>
+    <hyperlink ref="G91" r:id="rId77" display="https://freegenes.github.io/genbank/BBF10K_003323.gb" xr:uid="{AA77869A-3223-7F44-B358-1D64C4798AAA}"/>
+    <hyperlink ref="G92" r:id="rId78" display="https://freegenes.github.io/genbank/BBF10K_003324.gb" xr:uid="{3C5FABFE-EF99-2748-9F8A-3AE181F40722}"/>
+    <hyperlink ref="G93" r:id="rId79" display="https://freegenes.github.io/genbank/BBF10K_003325.gb" xr:uid="{182169C3-34ED-6644-AD8D-026D0175349A}"/>
+    <hyperlink ref="G94" r:id="rId80" display="https://freegenes.github.io/genbank/BBF10K_003326.gb" xr:uid="{CC08E01A-F5D6-4441-9660-0770844DAD79}"/>
+    <hyperlink ref="G95" r:id="rId81" display="https://freegenes.github.io/genbank/BBF10K_003327.gb" xr:uid="{2FB5E4AD-8DCD-1440-BB30-3D1083AC72E6}"/>
+    <hyperlink ref="G96" r:id="rId82" display="https://freegenes.github.io/genbank/BBF10K_003328.gb" xr:uid="{4D1242ED-DC29-0847-BF8D-B435FFBB8DD6}"/>
+    <hyperlink ref="G97" r:id="rId83" display="https://freegenes.github.io/genbank/BBF10K_003329.gb" xr:uid="{C10EFD59-A0AB-F146-96D6-449BE233AF4C}"/>
+    <hyperlink ref="G98" r:id="rId84" display="https://freegenes.github.io/genbank/BBF10K_003330.gb" xr:uid="{AE09611B-1C69-9048-B398-01DD25262534}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>